<commit_message>
# update trigger program.
</commit_message>
<xml_diff>
--- a/trace/trace.xlsx
+++ b/trace/trace.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="810" yWindow="3000" windowWidth="14295" windowHeight="7020"/>
+    <workbookView xWindow="810" yWindow="3000" windowWidth="14295" windowHeight="7020" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="00mgmemt" sheetId="2" r:id="rId1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="172">
   <si>
     <t>mgmemt.p</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -510,6 +510,182 @@
   <si>
     <t>CH</t>
     <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>tce_time</t>
+  </si>
+  <si>
+    <t>tce_tabrecid</t>
+  </si>
+  <si>
+    <t>tce_type</t>
+  </si>
+  <si>
+    <t>tce_table</t>
+  </si>
+  <si>
+    <t>tce_fld</t>
+  </si>
+  <si>
+    <t>tce_aval</t>
+  </si>
+  <si>
+    <t>tce_bval</t>
+  </si>
+  <si>
+    <t>tce_domain</t>
+  </si>
+  <si>
+    <t>tce_part</t>
+  </si>
+  <si>
+    <t>tce_site</t>
+  </si>
+  <si>
+    <t>tce_nbr</t>
+  </si>
+  <si>
+    <t>tce_host</t>
+  </si>
+  <si>
+    <t>tce_osuser</t>
+  </si>
+  <si>
+    <t>tce_userid</t>
+  </si>
+  <si>
+    <t>tce_date</t>
+  </si>
+  <si>
+    <t>tce_prog</t>
+  </si>
+  <si>
+    <t>tce_stack</t>
+  </si>
+  <si>
+    <t>tce_key0</t>
+  </si>
+  <si>
+    <t>tce_key1</t>
+  </si>
+  <si>
+    <t>tce_key2</t>
+  </si>
+  <si>
+    <t>tce_key3</t>
+  </si>
+  <si>
+    <t>tce_key4</t>
+  </si>
+  <si>
+    <t>tce_key5</t>
+  </si>
+  <si>
+    <t>tce_key6</t>
+  </si>
+  <si>
+    <t>tce_key7</t>
+  </si>
+  <si>
+    <t>tce_key8</t>
+  </si>
+  <si>
+    <t>tce_key9</t>
+  </si>
+  <si>
+    <t>tce_interface</t>
+  </si>
+  <si>
+    <t>INTERFACE_TYPE</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>type</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>ID</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>table</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>field</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>current</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>before</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>domain</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>part</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>site</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>number</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>host</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>date</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>time</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>program</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>STACKED_LABEL</t>
+  </si>
+  <si>
+    <t>xxtciq.p</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>表/字段跟踪程查询</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>xxtciq.p</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>tcenbr</t>
+  </si>
+  <si>
+    <t>RECID</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>tce_logindate</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>LOGIN_DATE</t>
+  </si>
+  <si>
+    <t>ENFORCE_OS_USER_ID</t>
   </si>
 </sst>
 </file>
@@ -924,13 +1100,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="4" topLeftCell="D5" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="3" ySplit="4" topLeftCell="D8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.25" defaultRowHeight="13.5"/>
@@ -1073,9 +1249,26 @@
         <v>116</v>
       </c>
     </row>
+    <row r="9" spans="1:9">
+      <c r="A9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9">
+        <v>6.1</v>
+      </c>
+      <c r="C9">
+        <v>11</v>
+      </c>
+      <c r="D9" t="s">
+        <v>165</v>
+      </c>
+      <c r="F9" t="s">
+        <v>166</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
-  <dataValidations count="4">
+  <dataValidations disablePrompts="1" count="4">
     <dataValidation type="list" imeMode="off" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H5:H65536">
       <formula1>".,~"</formula1>
     </dataValidation>
@@ -1103,7 +1296,7 @@
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C4" sqref="C4"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13" defaultRowHeight="13.5"/>
@@ -1770,12 +1963,12 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C31"/>
+  <dimension ref="A1:C61"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C4" sqref="C4"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -2309,6 +2502,336 @@
         <v>114</v>
       </c>
     </row>
+    <row r="32" spans="1:3">
+      <c r="A32" t="s">
+        <v>167</v>
+      </c>
+      <c r="B32" t="s">
+        <v>164</v>
+      </c>
+      <c r="C32" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" t="s">
+        <v>121</v>
+      </c>
+      <c r="B33" t="s">
+        <v>164</v>
+      </c>
+      <c r="C33" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" t="s">
+        <v>122</v>
+      </c>
+      <c r="B34" t="s">
+        <v>164</v>
+      </c>
+      <c r="C34" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" t="s">
+        <v>123</v>
+      </c>
+      <c r="B35" t="s">
+        <v>164</v>
+      </c>
+      <c r="C35" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" t="s">
+        <v>124</v>
+      </c>
+      <c r="B36" t="s">
+        <v>164</v>
+      </c>
+      <c r="C36" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" t="s">
+        <v>125</v>
+      </c>
+      <c r="B37" t="s">
+        <v>164</v>
+      </c>
+      <c r="C37" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" t="s">
+        <v>126</v>
+      </c>
+      <c r="B38" t="s">
+        <v>164</v>
+      </c>
+      <c r="C38" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" t="s">
+        <v>127</v>
+      </c>
+      <c r="B39" t="s">
+        <v>164</v>
+      </c>
+      <c r="C39" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" t="s">
+        <v>128</v>
+      </c>
+      <c r="B40" t="s">
+        <v>164</v>
+      </c>
+      <c r="C40" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" t="s">
+        <v>129</v>
+      </c>
+      <c r="B41" t="s">
+        <v>164</v>
+      </c>
+      <c r="C41" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" t="s">
+        <v>130</v>
+      </c>
+      <c r="B42" t="s">
+        <v>164</v>
+      </c>
+      <c r="C42" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43" t="s">
+        <v>131</v>
+      </c>
+      <c r="B43" t="s">
+        <v>164</v>
+      </c>
+      <c r="C43" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44" t="s">
+        <v>132</v>
+      </c>
+      <c r="B44" t="s">
+        <v>164</v>
+      </c>
+      <c r="C44" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45" t="s">
+        <v>133</v>
+      </c>
+      <c r="B45" t="s">
+        <v>164</v>
+      </c>
+      <c r="C45" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46" t="s">
+        <v>134</v>
+      </c>
+      <c r="B46" t="s">
+        <v>164</v>
+      </c>
+      <c r="C46" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="A47" t="s">
+        <v>120</v>
+      </c>
+      <c r="B47" t="s">
+        <v>164</v>
+      </c>
+      <c r="C47" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48" t="s">
+        <v>135</v>
+      </c>
+      <c r="B48" t="s">
+        <v>164</v>
+      </c>
+      <c r="C48" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49" t="s">
+        <v>136</v>
+      </c>
+      <c r="B49" t="s">
+        <v>164</v>
+      </c>
+      <c r="C49" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="A50" t="s">
+        <v>137</v>
+      </c>
+      <c r="B50" t="s">
+        <v>164</v>
+      </c>
+      <c r="C50" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51" t="s">
+        <v>138</v>
+      </c>
+      <c r="B51" t="s">
+        <v>164</v>
+      </c>
+      <c r="C51" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="A52" t="s">
+        <v>139</v>
+      </c>
+      <c r="B52" t="s">
+        <v>164</v>
+      </c>
+      <c r="C52" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3">
+      <c r="A53" t="s">
+        <v>140</v>
+      </c>
+      <c r="B53" t="s">
+        <v>164</v>
+      </c>
+      <c r="C53" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
+      <c r="A54" t="s">
+        <v>141</v>
+      </c>
+      <c r="B54" t="s">
+        <v>164</v>
+      </c>
+      <c r="C54" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
+      <c r="A55" t="s">
+        <v>142</v>
+      </c>
+      <c r="B55" t="s">
+        <v>164</v>
+      </c>
+      <c r="C55" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
+      <c r="A56" t="s">
+        <v>143</v>
+      </c>
+      <c r="B56" t="s">
+        <v>164</v>
+      </c>
+      <c r="C56" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3">
+      <c r="A57" t="s">
+        <v>144</v>
+      </c>
+      <c r="B57" t="s">
+        <v>164</v>
+      </c>
+      <c r="C57" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3">
+      <c r="A58" t="s">
+        <v>145</v>
+      </c>
+      <c r="B58" t="s">
+        <v>164</v>
+      </c>
+      <c r="C58" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3">
+      <c r="A59" t="s">
+        <v>146</v>
+      </c>
+      <c r="B59" t="s">
+        <v>164</v>
+      </c>
+      <c r="C59" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3">
+      <c r="A60" t="s">
+        <v>147</v>
+      </c>
+      <c r="B60" t="s">
+        <v>164</v>
+      </c>
+      <c r="C60" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3">
+      <c r="A61" t="s">
+        <v>169</v>
+      </c>
+      <c r="B61" t="s">
+        <v>164</v>
+      </c>
+      <c r="C61" t="s">
+        <v>170</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
# fix trace bug.
</commit_message>
<xml_diff>
--- a/trace/trace.xlsx
+++ b/trace/trace.xlsx
@@ -1100,6 +1100,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1291,6 +1292,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -1963,12 +1965,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:C61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C4" sqref="C4"/>
-      <selection pane="bottomLeft" activeCell="C46" sqref="C46"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -2840,6 +2843,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
+ add yeebo first program(wo maintenance).
</commit_message>
<xml_diff>
--- a/trace/trace.xlsx
+++ b/trace/trace.xlsx
@@ -616,10 +616,6 @@
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
-    <t>current</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
     <t>before</t>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
@@ -686,6 +682,10 @@
   </si>
   <si>
     <t>ENFORCE_OS_USER_ID</t>
+  </si>
+  <si>
+    <t>after</t>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1261,10 +1261,10 @@
         <v>11</v>
       </c>
       <c r="D9" t="s">
+        <v>164</v>
+      </c>
+      <c r="F9" t="s">
         <v>165</v>
-      </c>
-      <c r="F9" t="s">
-        <v>166</v>
       </c>
     </row>
   </sheetData>
@@ -1971,7 +1971,7 @@
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C4" sqref="C4"/>
-      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -2507,10 +2507,10 @@
     </row>
     <row r="32" spans="1:3">
       <c r="A32" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B32" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C32" t="s">
         <v>150</v>
@@ -2521,10 +2521,10 @@
         <v>121</v>
       </c>
       <c r="B33" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C33" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="34" spans="1:3">
@@ -2532,7 +2532,7 @@
         <v>122</v>
       </c>
       <c r="B34" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C34" t="s">
         <v>149</v>
@@ -2543,7 +2543,7 @@
         <v>123</v>
       </c>
       <c r="B35" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C35" t="s">
         <v>151</v>
@@ -2554,7 +2554,7 @@
         <v>124</v>
       </c>
       <c r="B36" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C36" t="s">
         <v>152</v>
@@ -2565,10 +2565,10 @@
         <v>125</v>
       </c>
       <c r="B37" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C37" t="s">
-        <v>153</v>
+        <v>171</v>
       </c>
     </row>
     <row r="38" spans="1:3">
@@ -2576,10 +2576,10 @@
         <v>126</v>
       </c>
       <c r="B38" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C38" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="39" spans="1:3">
@@ -2587,10 +2587,10 @@
         <v>127</v>
       </c>
       <c r="B39" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C39" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="40" spans="1:3">
@@ -2598,10 +2598,10 @@
         <v>128</v>
       </c>
       <c r="B40" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C40" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="41" spans="1:3">
@@ -2609,10 +2609,10 @@
         <v>129</v>
       </c>
       <c r="B41" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C41" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="42" spans="1:3">
@@ -2620,10 +2620,10 @@
         <v>130</v>
       </c>
       <c r="B42" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C42" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="43" spans="1:3">
@@ -2631,10 +2631,10 @@
         <v>131</v>
       </c>
       <c r="B43" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C43" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="44" spans="1:3">
@@ -2642,10 +2642,10 @@
         <v>132</v>
       </c>
       <c r="B44" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C44" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="45" spans="1:3">
@@ -2653,7 +2653,7 @@
         <v>133</v>
       </c>
       <c r="B45" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C45" t="s">
         <v>64</v>
@@ -2664,10 +2664,10 @@
         <v>134</v>
       </c>
       <c r="B46" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C46" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="47" spans="1:3">
@@ -2675,10 +2675,10 @@
         <v>120</v>
       </c>
       <c r="B47" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C47" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="48" spans="1:3">
@@ -2686,10 +2686,10 @@
         <v>135</v>
       </c>
       <c r="B48" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C48" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="49" spans="1:3">
@@ -2697,10 +2697,10 @@
         <v>136</v>
       </c>
       <c r="B49" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C49" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="50" spans="1:3">
@@ -2708,7 +2708,7 @@
         <v>137</v>
       </c>
       <c r="B50" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C50" t="s">
         <v>105</v>
@@ -2719,7 +2719,7 @@
         <v>138</v>
       </c>
       <c r="B51" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C51" t="s">
         <v>106</v>
@@ -2730,7 +2730,7 @@
         <v>139</v>
       </c>
       <c r="B52" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C52" t="s">
         <v>107</v>
@@ -2741,7 +2741,7 @@
         <v>140</v>
       </c>
       <c r="B53" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C53" t="s">
         <v>108</v>
@@ -2752,7 +2752,7 @@
         <v>141</v>
       </c>
       <c r="B54" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C54" t="s">
         <v>109</v>
@@ -2763,7 +2763,7 @@
         <v>142</v>
       </c>
       <c r="B55" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C55" t="s">
         <v>110</v>
@@ -2774,7 +2774,7 @@
         <v>143</v>
       </c>
       <c r="B56" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C56" t="s">
         <v>111</v>
@@ -2785,7 +2785,7 @@
         <v>144</v>
       </c>
       <c r="B57" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C57" t="s">
         <v>112</v>
@@ -2796,7 +2796,7 @@
         <v>145</v>
       </c>
       <c r="B58" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C58" t="s">
         <v>113</v>
@@ -2807,7 +2807,7 @@
         <v>146</v>
       </c>
       <c r="B59" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C59" t="s">
         <v>114</v>
@@ -2818,7 +2818,7 @@
         <v>147</v>
       </c>
       <c r="B60" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C60" t="s">
         <v>148</v>
@@ -2826,13 +2826,13 @@
     </row>
     <row r="61" spans="1:3">
       <c r="A61" t="s">
+        <v>168</v>
+      </c>
+      <c r="B61" t="s">
+        <v>163</v>
+      </c>
+      <c r="C61" t="s">
         <v>169</v>
-      </c>
-      <c r="B61" t="s">
-        <v>164</v>
-      </c>
-      <c r="C61" t="s">
-        <v>170</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
# add xxtcrp.p /*tce report*/
</commit_message>
<xml_diff>
--- a/trace/trace.xlsx
+++ b/trace/trace.xlsx
@@ -652,9 +652,6 @@
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
-    <t>STACKED_LABEL</t>
-  </si>
-  <si>
     <t>xxtciq.p</t>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
@@ -686,6 +683,9 @@
   <si>
     <t>after</t>
     <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>PROGRAM_STACK</t>
   </si>
 </sst>
 </file>
@@ -1261,10 +1261,10 @@
         <v>11</v>
       </c>
       <c r="D9" t="s">
+        <v>163</v>
+      </c>
+      <c r="F9" t="s">
         <v>164</v>
-      </c>
-      <c r="F9" t="s">
-        <v>165</v>
       </c>
     </row>
   </sheetData>
@@ -1969,9 +1969,9 @@
   <dimension ref="A1:C61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="4" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C4" sqref="C4"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="C49" sqref="C49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -2507,10 +2507,10 @@
     </row>
     <row r="32" spans="1:3">
       <c r="A32" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B32" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C32" t="s">
         <v>150</v>
@@ -2521,10 +2521,10 @@
         <v>121</v>
       </c>
       <c r="B33" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C33" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="34" spans="1:3">
@@ -2532,7 +2532,7 @@
         <v>122</v>
       </c>
       <c r="B34" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C34" t="s">
         <v>149</v>
@@ -2543,7 +2543,7 @@
         <v>123</v>
       </c>
       <c r="B35" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C35" t="s">
         <v>151</v>
@@ -2554,7 +2554,7 @@
         <v>124</v>
       </c>
       <c r="B36" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C36" t="s">
         <v>152</v>
@@ -2565,10 +2565,10 @@
         <v>125</v>
       </c>
       <c r="B37" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C37" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="38" spans="1:3">
@@ -2576,7 +2576,7 @@
         <v>126</v>
       </c>
       <c r="B38" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C38" t="s">
         <v>153</v>
@@ -2587,7 +2587,7 @@
         <v>127</v>
       </c>
       <c r="B39" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C39" t="s">
         <v>154</v>
@@ -2598,7 +2598,7 @@
         <v>128</v>
       </c>
       <c r="B40" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C40" t="s">
         <v>155</v>
@@ -2609,7 +2609,7 @@
         <v>129</v>
       </c>
       <c r="B41" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C41" t="s">
         <v>156</v>
@@ -2620,7 +2620,7 @@
         <v>130</v>
       </c>
       <c r="B42" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C42" t="s">
         <v>157</v>
@@ -2631,7 +2631,7 @@
         <v>131</v>
       </c>
       <c r="B43" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C43" t="s">
         <v>158</v>
@@ -2642,10 +2642,10 @@
         <v>132</v>
       </c>
       <c r="B44" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C44" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="45" spans="1:3">
@@ -2653,7 +2653,7 @@
         <v>133</v>
       </c>
       <c r="B45" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C45" t="s">
         <v>64</v>
@@ -2664,7 +2664,7 @@
         <v>134</v>
       </c>
       <c r="B46" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C46" t="s">
         <v>159</v>
@@ -2675,7 +2675,7 @@
         <v>120</v>
       </c>
       <c r="B47" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C47" t="s">
         <v>160</v>
@@ -2686,7 +2686,7 @@
         <v>135</v>
       </c>
       <c r="B48" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C48" t="s">
         <v>161</v>
@@ -2697,10 +2697,10 @@
         <v>136</v>
       </c>
       <c r="B49" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C49" t="s">
-        <v>162</v>
+        <v>171</v>
       </c>
     </row>
     <row r="50" spans="1:3">
@@ -2708,7 +2708,7 @@
         <v>137</v>
       </c>
       <c r="B50" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C50" t="s">
         <v>105</v>
@@ -2719,7 +2719,7 @@
         <v>138</v>
       </c>
       <c r="B51" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C51" t="s">
         <v>106</v>
@@ -2730,7 +2730,7 @@
         <v>139</v>
       </c>
       <c r="B52" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C52" t="s">
         <v>107</v>
@@ -2741,7 +2741,7 @@
         <v>140</v>
       </c>
       <c r="B53" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C53" t="s">
         <v>108</v>
@@ -2752,7 +2752,7 @@
         <v>141</v>
       </c>
       <c r="B54" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C54" t="s">
         <v>109</v>
@@ -2763,7 +2763,7 @@
         <v>142</v>
       </c>
       <c r="B55" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C55" t="s">
         <v>110</v>
@@ -2774,7 +2774,7 @@
         <v>143</v>
       </c>
       <c r="B56" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C56" t="s">
         <v>111</v>
@@ -2785,7 +2785,7 @@
         <v>144</v>
       </c>
       <c r="B57" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C57" t="s">
         <v>112</v>
@@ -2796,7 +2796,7 @@
         <v>145</v>
       </c>
       <c r="B58" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C58" t="s">
         <v>113</v>
@@ -2807,7 +2807,7 @@
         <v>146</v>
       </c>
       <c r="B59" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C59" t="s">
         <v>114</v>
@@ -2818,7 +2818,7 @@
         <v>147</v>
       </c>
       <c r="B60" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C60" t="s">
         <v>148</v>
@@ -2826,13 +2826,13 @@
     </row>
     <row r="61" spans="1:3">
       <c r="A61" t="s">
+        <v>167</v>
+      </c>
+      <c r="B61" t="s">
+        <v>162</v>
+      </c>
+      <c r="C61" t="s">
         <v>168</v>
-      </c>
-      <c r="B61" t="s">
-        <v>163</v>
-      </c>
-      <c r="C61" t="s">
-        <v>169</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
# add report xxtcrp.
</commit_message>
<xml_diff>
--- a/trace/trace.xlsx
+++ b/trace/trace.xlsx
@@ -4,13 +4,14 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="810" yWindow="3000" windowWidth="14295" windowHeight="7020" activeTab="2"/>
+    <workbookView xWindow="4860" yWindow="1485" windowWidth="14295" windowHeight="7020" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="00mgmemt" sheetId="2" r:id="rId1"/>
     <sheet name="11gplblmt.p" sheetId="3" r:id="rId2"/>
     <sheet name="12gplbldmt" sheetId="4" r:id="rId3"/>
     <sheet name="05mgmsgmt.p" sheetId="5" r:id="rId4"/>
+    <sheet name="06mgdlfhmt.p" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
@@ -62,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="199">
   <si>
     <t>mgmemt.p</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -686,13 +687,130 @@
   </si>
   <si>
     <t>PROGRAM_STACK</t>
+  </si>
+  <si>
+    <t>-</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3/3-N</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3/2-N</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3/1-C24</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2/1-C12</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1/3-C10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1/2-C32</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1/1-C8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>查找项</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>查找从行开始</t>
+  </si>
+  <si>
+    <t>描述</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>要执行的过程</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>呼叫过程</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>字段名称</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>详细查询/查找</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>flh_down</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>flh_y</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>flh_desc</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>exec</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>call_pgm</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fieldname</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>l_drl_lookup</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>36.20.1 详细查询查询维护</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mgdlfhmt.p</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>t</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>bl</t>
+    </r>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>xxlu910.p</t>
+  </si>
+  <si>
+    <t>TRACE_ACTIVE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -737,8 +855,15 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -769,6 +894,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -779,12 +916,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -806,9 +946,25 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="常规 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1107,7 +1263,7 @@
       <pane xSplit="3" ySplit="4" topLeftCell="D8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="F10" sqref="F10"/>
+      <selection pane="bottomRight" activeCell="J21" sqref="A18:J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.25" defaultRowHeight="13.5"/>
@@ -1968,7 +2124,7 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:C61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="4" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C4" sqref="C4"/>
       <selection pane="bottomLeft" activeCell="C49" sqref="C49"/>
@@ -2909,4 +3065,143 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
+      <selection pane="bottomRight" activeCell="E5" sqref="E5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5"/>
+  <cols>
+    <col min="1" max="1" width="14.125" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.375" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.5" style="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9" style="7"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>192</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>191</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>189</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>188</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="7" t="s">
+        <v>186</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>183</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>178</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>176</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>174</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>196</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="F5" s="7">
+        <v>7</v>
+      </c>
+      <c r="G5" s="7">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="6" type="noConversion"/>
+  <dataValidations count="3">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="请输入数字" prompt="6" sqref="G5:G65536 JC5:JC65536 SY5:SY65536 ACU5:ACU65536 AMQ5:AMQ65536 AWM5:AWM65536 BGI5:BGI65536 BQE5:BQE65536 CAA5:CAA65536 CJW5:CJW65536 CTS5:CTS65536 DDO5:DDO65536 DNK5:DNK65536 DXG5:DXG65536 EHC5:EHC65536 EQY5:EQY65536 FAU5:FAU65536 FKQ5:FKQ65536 FUM5:FUM65536 GEI5:GEI65536 GOE5:GOE65536 GYA5:GYA65536 HHW5:HHW65536 HRS5:HRS65536 IBO5:IBO65536 ILK5:ILK65536 IVG5:IVG65536 JFC5:JFC65536 JOY5:JOY65536 JYU5:JYU65536 KIQ5:KIQ65536 KSM5:KSM65536 LCI5:LCI65536 LME5:LME65536 LWA5:LWA65536 MFW5:MFW65536 MPS5:MPS65536 MZO5:MZO65536 NJK5:NJK65536 NTG5:NTG65536 ODC5:ODC65536 OMY5:OMY65536 OWU5:OWU65536 PGQ5:PGQ65536 PQM5:PQM65536 QAI5:QAI65536 QKE5:QKE65536 QUA5:QUA65536 RDW5:RDW65536 RNS5:RNS65536 RXO5:RXO65536 SHK5:SHK65536 SRG5:SRG65536 TBC5:TBC65536 TKY5:TKY65536 TUU5:TUU65536 UEQ5:UEQ65536 UOM5:UOM65536 UYI5:UYI65536 VIE5:VIE65536 VSA5:VSA65536 WBW5:WBW65536 WLS5:WLS65536 WVO5:WVO65536 G65541:G131072 JC65541:JC131072 SY65541:SY131072 ACU65541:ACU131072 AMQ65541:AMQ131072 AWM65541:AWM131072 BGI65541:BGI131072 BQE65541:BQE131072 CAA65541:CAA131072 CJW65541:CJW131072 CTS65541:CTS131072 DDO65541:DDO131072 DNK65541:DNK131072 DXG65541:DXG131072 EHC65541:EHC131072 EQY65541:EQY131072 FAU65541:FAU131072 FKQ65541:FKQ131072 FUM65541:FUM131072 GEI65541:GEI131072 GOE65541:GOE131072 GYA65541:GYA131072 HHW65541:HHW131072 HRS65541:HRS131072 IBO65541:IBO131072 ILK65541:ILK131072 IVG65541:IVG131072 JFC65541:JFC131072 JOY65541:JOY131072 JYU65541:JYU131072 KIQ65541:KIQ131072 KSM65541:KSM131072 LCI65541:LCI131072 LME65541:LME131072 LWA65541:LWA131072 MFW65541:MFW131072 MPS65541:MPS131072 MZO65541:MZO131072 NJK65541:NJK131072 NTG65541:NTG131072 ODC65541:ODC131072 OMY65541:OMY131072 OWU65541:OWU131072 PGQ65541:PGQ131072 PQM65541:PQM131072 QAI65541:QAI131072 QKE65541:QKE131072 QUA65541:QUA131072 RDW65541:RDW131072 RNS65541:RNS131072 RXO65541:RXO131072 SHK65541:SHK131072 SRG65541:SRG131072 TBC65541:TBC131072 TKY65541:TKY131072 TUU65541:TUU131072 UEQ65541:UEQ131072 UOM65541:UOM131072 UYI65541:UYI131072 VIE65541:VIE131072 VSA65541:VSA131072 WBW65541:WBW131072 WLS65541:WLS131072 WVO65541:WVO131072 G131077:G196608 JC131077:JC196608 SY131077:SY196608 ACU131077:ACU196608 AMQ131077:AMQ196608 AWM131077:AWM196608 BGI131077:BGI196608 BQE131077:BQE196608 CAA131077:CAA196608 CJW131077:CJW196608 CTS131077:CTS196608 DDO131077:DDO196608 DNK131077:DNK196608 DXG131077:DXG196608 EHC131077:EHC196608 EQY131077:EQY196608 FAU131077:FAU196608 FKQ131077:FKQ196608 FUM131077:FUM196608 GEI131077:GEI196608 GOE131077:GOE196608 GYA131077:GYA196608 HHW131077:HHW196608 HRS131077:HRS196608 IBO131077:IBO196608 ILK131077:ILK196608 IVG131077:IVG196608 JFC131077:JFC196608 JOY131077:JOY196608 JYU131077:JYU196608 KIQ131077:KIQ196608 KSM131077:KSM196608 LCI131077:LCI196608 LME131077:LME196608 LWA131077:LWA196608 MFW131077:MFW196608 MPS131077:MPS196608 MZO131077:MZO196608 NJK131077:NJK196608 NTG131077:NTG196608 ODC131077:ODC196608 OMY131077:OMY196608 OWU131077:OWU196608 PGQ131077:PGQ196608 PQM131077:PQM196608 QAI131077:QAI196608 QKE131077:QKE196608 QUA131077:QUA196608 RDW131077:RDW196608 RNS131077:RNS196608 RXO131077:RXO196608 SHK131077:SHK196608 SRG131077:SRG196608 TBC131077:TBC196608 TKY131077:TKY196608 TUU131077:TUU196608 UEQ131077:UEQ196608 UOM131077:UOM196608 UYI131077:UYI196608 VIE131077:VIE196608 VSA131077:VSA196608 WBW131077:WBW196608 WLS131077:WLS196608 WVO131077:WVO196608 G196613:G262144 JC196613:JC262144 SY196613:SY262144 ACU196613:ACU262144 AMQ196613:AMQ262144 AWM196613:AWM262144 BGI196613:BGI262144 BQE196613:BQE262144 CAA196613:CAA262144 CJW196613:CJW262144 CTS196613:CTS262144 DDO196613:DDO262144 DNK196613:DNK262144 DXG196613:DXG262144 EHC196613:EHC262144 EQY196613:EQY262144 FAU196613:FAU262144 FKQ196613:FKQ262144 FUM196613:FUM262144 GEI196613:GEI262144 GOE196613:GOE262144 GYA196613:GYA262144 HHW196613:HHW262144 HRS196613:HRS262144 IBO196613:IBO262144 ILK196613:ILK262144 IVG196613:IVG262144 JFC196613:JFC262144 JOY196613:JOY262144 JYU196613:JYU262144 KIQ196613:KIQ262144 KSM196613:KSM262144 LCI196613:LCI262144 LME196613:LME262144 LWA196613:LWA262144 MFW196613:MFW262144 MPS196613:MPS262144 MZO196613:MZO262144 NJK196613:NJK262144 NTG196613:NTG262144 ODC196613:ODC262144 OMY196613:OMY262144 OWU196613:OWU262144 PGQ196613:PGQ262144 PQM196613:PQM262144 QAI196613:QAI262144 QKE196613:QKE262144 QUA196613:QUA262144 RDW196613:RDW262144 RNS196613:RNS262144 RXO196613:RXO262144 SHK196613:SHK262144 SRG196613:SRG262144 TBC196613:TBC262144 TKY196613:TKY262144 TUU196613:TUU262144 UEQ196613:UEQ262144 UOM196613:UOM262144 UYI196613:UYI262144 VIE196613:VIE262144 VSA196613:VSA262144 WBW196613:WBW262144 WLS196613:WLS262144 WVO196613:WVO262144 G262149:G327680 JC262149:JC327680 SY262149:SY327680 ACU262149:ACU327680 AMQ262149:AMQ327680 AWM262149:AWM327680 BGI262149:BGI327680 BQE262149:BQE327680 CAA262149:CAA327680 CJW262149:CJW327680 CTS262149:CTS327680 DDO262149:DDO327680 DNK262149:DNK327680 DXG262149:DXG327680 EHC262149:EHC327680 EQY262149:EQY327680 FAU262149:FAU327680 FKQ262149:FKQ327680 FUM262149:FUM327680 GEI262149:GEI327680 GOE262149:GOE327680 GYA262149:GYA327680 HHW262149:HHW327680 HRS262149:HRS327680 IBO262149:IBO327680 ILK262149:ILK327680 IVG262149:IVG327680 JFC262149:JFC327680 JOY262149:JOY327680 JYU262149:JYU327680 KIQ262149:KIQ327680 KSM262149:KSM327680 LCI262149:LCI327680 LME262149:LME327680 LWA262149:LWA327680 MFW262149:MFW327680 MPS262149:MPS327680 MZO262149:MZO327680 NJK262149:NJK327680 NTG262149:NTG327680 ODC262149:ODC327680 OMY262149:OMY327680 OWU262149:OWU327680 PGQ262149:PGQ327680 PQM262149:PQM327680 QAI262149:QAI327680 QKE262149:QKE327680 QUA262149:QUA327680 RDW262149:RDW327680 RNS262149:RNS327680 RXO262149:RXO327680 SHK262149:SHK327680 SRG262149:SRG327680 TBC262149:TBC327680 TKY262149:TKY327680 TUU262149:TUU327680 UEQ262149:UEQ327680 UOM262149:UOM327680 UYI262149:UYI327680 VIE262149:VIE327680 VSA262149:VSA327680 WBW262149:WBW327680 WLS262149:WLS327680 WVO262149:WVO327680 G327685:G393216 JC327685:JC393216 SY327685:SY393216 ACU327685:ACU393216 AMQ327685:AMQ393216 AWM327685:AWM393216 BGI327685:BGI393216 BQE327685:BQE393216 CAA327685:CAA393216 CJW327685:CJW393216 CTS327685:CTS393216 DDO327685:DDO393216 DNK327685:DNK393216 DXG327685:DXG393216 EHC327685:EHC393216 EQY327685:EQY393216 FAU327685:FAU393216 FKQ327685:FKQ393216 FUM327685:FUM393216 GEI327685:GEI393216 GOE327685:GOE393216 GYA327685:GYA393216 HHW327685:HHW393216 HRS327685:HRS393216 IBO327685:IBO393216 ILK327685:ILK393216 IVG327685:IVG393216 JFC327685:JFC393216 JOY327685:JOY393216 JYU327685:JYU393216 KIQ327685:KIQ393216 KSM327685:KSM393216 LCI327685:LCI393216 LME327685:LME393216 LWA327685:LWA393216 MFW327685:MFW393216 MPS327685:MPS393216 MZO327685:MZO393216 NJK327685:NJK393216 NTG327685:NTG393216 ODC327685:ODC393216 OMY327685:OMY393216 OWU327685:OWU393216 PGQ327685:PGQ393216 PQM327685:PQM393216 QAI327685:QAI393216 QKE327685:QKE393216 QUA327685:QUA393216 RDW327685:RDW393216 RNS327685:RNS393216 RXO327685:RXO393216 SHK327685:SHK393216 SRG327685:SRG393216 TBC327685:TBC393216 TKY327685:TKY393216 TUU327685:TUU393216 UEQ327685:UEQ393216 UOM327685:UOM393216 UYI327685:UYI393216 VIE327685:VIE393216 VSA327685:VSA393216 WBW327685:WBW393216 WLS327685:WLS393216 WVO327685:WVO393216 G393221:G458752 JC393221:JC458752 SY393221:SY458752 ACU393221:ACU458752 AMQ393221:AMQ458752 AWM393221:AWM458752 BGI393221:BGI458752 BQE393221:BQE458752 CAA393221:CAA458752 CJW393221:CJW458752 CTS393221:CTS458752 DDO393221:DDO458752 DNK393221:DNK458752 DXG393221:DXG458752 EHC393221:EHC458752 EQY393221:EQY458752 FAU393221:FAU458752 FKQ393221:FKQ458752 FUM393221:FUM458752 GEI393221:GEI458752 GOE393221:GOE458752 GYA393221:GYA458752 HHW393221:HHW458752 HRS393221:HRS458752 IBO393221:IBO458752 ILK393221:ILK458752 IVG393221:IVG458752 JFC393221:JFC458752 JOY393221:JOY458752 JYU393221:JYU458752 KIQ393221:KIQ458752 KSM393221:KSM458752 LCI393221:LCI458752 LME393221:LME458752 LWA393221:LWA458752 MFW393221:MFW458752 MPS393221:MPS458752 MZO393221:MZO458752 NJK393221:NJK458752 NTG393221:NTG458752 ODC393221:ODC458752 OMY393221:OMY458752 OWU393221:OWU458752 PGQ393221:PGQ458752 PQM393221:PQM458752 QAI393221:QAI458752 QKE393221:QKE458752 QUA393221:QUA458752 RDW393221:RDW458752 RNS393221:RNS458752 RXO393221:RXO458752 SHK393221:SHK458752 SRG393221:SRG458752 TBC393221:TBC458752 TKY393221:TKY458752 TUU393221:TUU458752 UEQ393221:UEQ458752 UOM393221:UOM458752 UYI393221:UYI458752 VIE393221:VIE458752 VSA393221:VSA458752 WBW393221:WBW458752 WLS393221:WLS458752 WVO393221:WVO458752 G458757:G524288 JC458757:JC524288 SY458757:SY524288 ACU458757:ACU524288 AMQ458757:AMQ524288 AWM458757:AWM524288 BGI458757:BGI524288 BQE458757:BQE524288 CAA458757:CAA524288 CJW458757:CJW524288 CTS458757:CTS524288 DDO458757:DDO524288 DNK458757:DNK524288 DXG458757:DXG524288 EHC458757:EHC524288 EQY458757:EQY524288 FAU458757:FAU524288 FKQ458757:FKQ524288 FUM458757:FUM524288 GEI458757:GEI524288 GOE458757:GOE524288 GYA458757:GYA524288 HHW458757:HHW524288 HRS458757:HRS524288 IBO458757:IBO524288 ILK458757:ILK524288 IVG458757:IVG524288 JFC458757:JFC524288 JOY458757:JOY524288 JYU458757:JYU524288 KIQ458757:KIQ524288 KSM458757:KSM524288 LCI458757:LCI524288 LME458757:LME524288 LWA458757:LWA524288 MFW458757:MFW524288 MPS458757:MPS524288 MZO458757:MZO524288 NJK458757:NJK524288 NTG458757:NTG524288 ODC458757:ODC524288 OMY458757:OMY524288 OWU458757:OWU524288 PGQ458757:PGQ524288 PQM458757:PQM524288 QAI458757:QAI524288 QKE458757:QKE524288 QUA458757:QUA524288 RDW458757:RDW524288 RNS458757:RNS524288 RXO458757:RXO524288 SHK458757:SHK524288 SRG458757:SRG524288 TBC458757:TBC524288 TKY458757:TKY524288 TUU458757:TUU524288 UEQ458757:UEQ524288 UOM458757:UOM524288 UYI458757:UYI524288 VIE458757:VIE524288 VSA458757:VSA524288 WBW458757:WBW524288 WLS458757:WLS524288 WVO458757:WVO524288 G524293:G589824 JC524293:JC589824 SY524293:SY589824 ACU524293:ACU589824 AMQ524293:AMQ589824 AWM524293:AWM589824 BGI524293:BGI589824 BQE524293:BQE589824 CAA524293:CAA589824 CJW524293:CJW589824 CTS524293:CTS589824 DDO524293:DDO589824 DNK524293:DNK589824 DXG524293:DXG589824 EHC524293:EHC589824 EQY524293:EQY589824 FAU524293:FAU589824 FKQ524293:FKQ589824 FUM524293:FUM589824 GEI524293:GEI589824 GOE524293:GOE589824 GYA524293:GYA589824 HHW524293:HHW589824 HRS524293:HRS589824 IBO524293:IBO589824 ILK524293:ILK589824 IVG524293:IVG589824 JFC524293:JFC589824 JOY524293:JOY589824 JYU524293:JYU589824 KIQ524293:KIQ589824 KSM524293:KSM589824 LCI524293:LCI589824 LME524293:LME589824 LWA524293:LWA589824 MFW524293:MFW589824 MPS524293:MPS589824 MZO524293:MZO589824 NJK524293:NJK589824 NTG524293:NTG589824 ODC524293:ODC589824 OMY524293:OMY589824 OWU524293:OWU589824 PGQ524293:PGQ589824 PQM524293:PQM589824 QAI524293:QAI589824 QKE524293:QKE589824 QUA524293:QUA589824 RDW524293:RDW589824 RNS524293:RNS589824 RXO524293:RXO589824 SHK524293:SHK589824 SRG524293:SRG589824 TBC524293:TBC589824 TKY524293:TKY589824 TUU524293:TUU589824 UEQ524293:UEQ589824 UOM524293:UOM589824 UYI524293:UYI589824 VIE524293:VIE589824 VSA524293:VSA589824 WBW524293:WBW589824 WLS524293:WLS589824 WVO524293:WVO589824 G589829:G655360 JC589829:JC655360 SY589829:SY655360 ACU589829:ACU655360 AMQ589829:AMQ655360 AWM589829:AWM655360 BGI589829:BGI655360 BQE589829:BQE655360 CAA589829:CAA655360 CJW589829:CJW655360 CTS589829:CTS655360 DDO589829:DDO655360 DNK589829:DNK655360 DXG589829:DXG655360 EHC589829:EHC655360 EQY589829:EQY655360 FAU589829:FAU655360 FKQ589829:FKQ655360 FUM589829:FUM655360 GEI589829:GEI655360 GOE589829:GOE655360 GYA589829:GYA655360 HHW589829:HHW655360 HRS589829:HRS655360 IBO589829:IBO655360 ILK589829:ILK655360 IVG589829:IVG655360 JFC589829:JFC655360 JOY589829:JOY655360 JYU589829:JYU655360 KIQ589829:KIQ655360 KSM589829:KSM655360 LCI589829:LCI655360 LME589829:LME655360 LWA589829:LWA655360 MFW589829:MFW655360 MPS589829:MPS655360 MZO589829:MZO655360 NJK589829:NJK655360 NTG589829:NTG655360 ODC589829:ODC655360 OMY589829:OMY655360 OWU589829:OWU655360 PGQ589829:PGQ655360 PQM589829:PQM655360 QAI589829:QAI655360 QKE589829:QKE655360 QUA589829:QUA655360 RDW589829:RDW655360 RNS589829:RNS655360 RXO589829:RXO655360 SHK589829:SHK655360 SRG589829:SRG655360 TBC589829:TBC655360 TKY589829:TKY655360 TUU589829:TUU655360 UEQ589829:UEQ655360 UOM589829:UOM655360 UYI589829:UYI655360 VIE589829:VIE655360 VSA589829:VSA655360 WBW589829:WBW655360 WLS589829:WLS655360 WVO589829:WVO655360 G655365:G720896 JC655365:JC720896 SY655365:SY720896 ACU655365:ACU720896 AMQ655365:AMQ720896 AWM655365:AWM720896 BGI655365:BGI720896 BQE655365:BQE720896 CAA655365:CAA720896 CJW655365:CJW720896 CTS655365:CTS720896 DDO655365:DDO720896 DNK655365:DNK720896 DXG655365:DXG720896 EHC655365:EHC720896 EQY655365:EQY720896 FAU655365:FAU720896 FKQ655365:FKQ720896 FUM655365:FUM720896 GEI655365:GEI720896 GOE655365:GOE720896 GYA655365:GYA720896 HHW655365:HHW720896 HRS655365:HRS720896 IBO655365:IBO720896 ILK655365:ILK720896 IVG655365:IVG720896 JFC655365:JFC720896 JOY655365:JOY720896 JYU655365:JYU720896 KIQ655365:KIQ720896 KSM655365:KSM720896 LCI655365:LCI720896 LME655365:LME720896 LWA655365:LWA720896 MFW655365:MFW720896 MPS655365:MPS720896 MZO655365:MZO720896 NJK655365:NJK720896 NTG655365:NTG720896 ODC655365:ODC720896 OMY655365:OMY720896 OWU655365:OWU720896 PGQ655365:PGQ720896 PQM655365:PQM720896 QAI655365:QAI720896 QKE655365:QKE720896 QUA655365:QUA720896 RDW655365:RDW720896 RNS655365:RNS720896 RXO655365:RXO720896 SHK655365:SHK720896 SRG655365:SRG720896 TBC655365:TBC720896 TKY655365:TKY720896 TUU655365:TUU720896 UEQ655365:UEQ720896 UOM655365:UOM720896 UYI655365:UYI720896 VIE655365:VIE720896 VSA655365:VSA720896 WBW655365:WBW720896 WLS655365:WLS720896 WVO655365:WVO720896 G720901:G786432 JC720901:JC786432 SY720901:SY786432 ACU720901:ACU786432 AMQ720901:AMQ786432 AWM720901:AWM786432 BGI720901:BGI786432 BQE720901:BQE786432 CAA720901:CAA786432 CJW720901:CJW786432 CTS720901:CTS786432 DDO720901:DDO786432 DNK720901:DNK786432 DXG720901:DXG786432 EHC720901:EHC786432 EQY720901:EQY786432 FAU720901:FAU786432 FKQ720901:FKQ786432 FUM720901:FUM786432 GEI720901:GEI786432 GOE720901:GOE786432 GYA720901:GYA786432 HHW720901:HHW786432 HRS720901:HRS786432 IBO720901:IBO786432 ILK720901:ILK786432 IVG720901:IVG786432 JFC720901:JFC786432 JOY720901:JOY786432 JYU720901:JYU786432 KIQ720901:KIQ786432 KSM720901:KSM786432 LCI720901:LCI786432 LME720901:LME786432 LWA720901:LWA786432 MFW720901:MFW786432 MPS720901:MPS786432 MZO720901:MZO786432 NJK720901:NJK786432 NTG720901:NTG786432 ODC720901:ODC786432 OMY720901:OMY786432 OWU720901:OWU786432 PGQ720901:PGQ786432 PQM720901:PQM786432 QAI720901:QAI786432 QKE720901:QKE786432 QUA720901:QUA786432 RDW720901:RDW786432 RNS720901:RNS786432 RXO720901:RXO786432 SHK720901:SHK786432 SRG720901:SRG786432 TBC720901:TBC786432 TKY720901:TKY786432 TUU720901:TUU786432 UEQ720901:UEQ786432 UOM720901:UOM786432 UYI720901:UYI786432 VIE720901:VIE786432 VSA720901:VSA786432 WBW720901:WBW786432 WLS720901:WLS786432 WVO720901:WVO786432 G786437:G851968 JC786437:JC851968 SY786437:SY851968 ACU786437:ACU851968 AMQ786437:AMQ851968 AWM786437:AWM851968 BGI786437:BGI851968 BQE786437:BQE851968 CAA786437:CAA851968 CJW786437:CJW851968 CTS786437:CTS851968 DDO786437:DDO851968 DNK786437:DNK851968 DXG786437:DXG851968 EHC786437:EHC851968 EQY786437:EQY851968 FAU786437:FAU851968 FKQ786437:FKQ851968 FUM786437:FUM851968 GEI786437:GEI851968 GOE786437:GOE851968 GYA786437:GYA851968 HHW786437:HHW851968 HRS786437:HRS851968 IBO786437:IBO851968 ILK786437:ILK851968 IVG786437:IVG851968 JFC786437:JFC851968 JOY786437:JOY851968 JYU786437:JYU851968 KIQ786437:KIQ851968 KSM786437:KSM851968 LCI786437:LCI851968 LME786437:LME851968 LWA786437:LWA851968 MFW786437:MFW851968 MPS786437:MPS851968 MZO786437:MZO851968 NJK786437:NJK851968 NTG786437:NTG851968 ODC786437:ODC851968 OMY786437:OMY851968 OWU786437:OWU851968 PGQ786437:PGQ851968 PQM786437:PQM851968 QAI786437:QAI851968 QKE786437:QKE851968 QUA786437:QUA851968 RDW786437:RDW851968 RNS786437:RNS851968 RXO786437:RXO851968 SHK786437:SHK851968 SRG786437:SRG851968 TBC786437:TBC851968 TKY786437:TKY851968 TUU786437:TUU851968 UEQ786437:UEQ851968 UOM786437:UOM851968 UYI786437:UYI851968 VIE786437:VIE851968 VSA786437:VSA851968 WBW786437:WBW851968 WLS786437:WLS851968 WVO786437:WVO851968 G851973:G917504 JC851973:JC917504 SY851973:SY917504 ACU851973:ACU917504 AMQ851973:AMQ917504 AWM851973:AWM917504 BGI851973:BGI917504 BQE851973:BQE917504 CAA851973:CAA917504 CJW851973:CJW917504 CTS851973:CTS917504 DDO851973:DDO917504 DNK851973:DNK917504 DXG851973:DXG917504 EHC851973:EHC917504 EQY851973:EQY917504 FAU851973:FAU917504 FKQ851973:FKQ917504 FUM851973:FUM917504 GEI851973:GEI917504 GOE851973:GOE917504 GYA851973:GYA917504 HHW851973:HHW917504 HRS851973:HRS917504 IBO851973:IBO917504 ILK851973:ILK917504 IVG851973:IVG917504 JFC851973:JFC917504 JOY851973:JOY917504 JYU851973:JYU917504 KIQ851973:KIQ917504 KSM851973:KSM917504 LCI851973:LCI917504 LME851973:LME917504 LWA851973:LWA917504 MFW851973:MFW917504 MPS851973:MPS917504 MZO851973:MZO917504 NJK851973:NJK917504 NTG851973:NTG917504 ODC851973:ODC917504 OMY851973:OMY917504 OWU851973:OWU917504 PGQ851973:PGQ917504 PQM851973:PQM917504 QAI851973:QAI917504 QKE851973:QKE917504 QUA851973:QUA917504 RDW851973:RDW917504 RNS851973:RNS917504 RXO851973:RXO917504 SHK851973:SHK917504 SRG851973:SRG917504 TBC851973:TBC917504 TKY851973:TKY917504 TUU851973:TUU917504 UEQ851973:UEQ917504 UOM851973:UOM917504 UYI851973:UYI917504 VIE851973:VIE917504 VSA851973:VSA917504 WBW851973:WBW917504 WLS851973:WLS917504 WVO851973:WVO917504 G917509:G983040 JC917509:JC983040 SY917509:SY983040 ACU917509:ACU983040 AMQ917509:AMQ983040 AWM917509:AWM983040 BGI917509:BGI983040 BQE917509:BQE983040 CAA917509:CAA983040 CJW917509:CJW983040 CTS917509:CTS983040 DDO917509:DDO983040 DNK917509:DNK983040 DXG917509:DXG983040 EHC917509:EHC983040 EQY917509:EQY983040 FAU917509:FAU983040 FKQ917509:FKQ983040 FUM917509:FUM983040 GEI917509:GEI983040 GOE917509:GOE983040 GYA917509:GYA983040 HHW917509:HHW983040 HRS917509:HRS983040 IBO917509:IBO983040 ILK917509:ILK983040 IVG917509:IVG983040 JFC917509:JFC983040 JOY917509:JOY983040 JYU917509:JYU983040 KIQ917509:KIQ983040 KSM917509:KSM983040 LCI917509:LCI983040 LME917509:LME983040 LWA917509:LWA983040 MFW917509:MFW983040 MPS917509:MPS983040 MZO917509:MZO983040 NJK917509:NJK983040 NTG917509:NTG983040 ODC917509:ODC983040 OMY917509:OMY983040 OWU917509:OWU983040 PGQ917509:PGQ983040 PQM917509:PQM983040 QAI917509:QAI983040 QKE917509:QKE983040 QUA917509:QUA983040 RDW917509:RDW983040 RNS917509:RNS983040 RXO917509:RXO983040 SHK917509:SHK983040 SRG917509:SRG983040 TBC917509:TBC983040 TKY917509:TKY983040 TUU917509:TUU983040 UEQ917509:UEQ983040 UOM917509:UOM983040 UYI917509:UYI983040 VIE917509:VIE983040 VSA917509:VSA983040 WBW917509:WBW983040 WLS917509:WLS983040 WVO917509:WVO983040 G983045:G1048576 JC983045:JC1048576 SY983045:SY1048576 ACU983045:ACU1048576 AMQ983045:AMQ1048576 AWM983045:AWM1048576 BGI983045:BGI1048576 BQE983045:BQE1048576 CAA983045:CAA1048576 CJW983045:CJW1048576 CTS983045:CTS1048576 DDO983045:DDO1048576 DNK983045:DNK1048576 DXG983045:DXG1048576 EHC983045:EHC1048576 EQY983045:EQY1048576 FAU983045:FAU1048576 FKQ983045:FKQ1048576 FUM983045:FUM1048576 GEI983045:GEI1048576 GOE983045:GOE1048576 GYA983045:GYA1048576 HHW983045:HHW1048576 HRS983045:HRS1048576 IBO983045:IBO1048576 ILK983045:ILK1048576 IVG983045:IVG1048576 JFC983045:JFC1048576 JOY983045:JOY1048576 JYU983045:JYU1048576 KIQ983045:KIQ1048576 KSM983045:KSM1048576 LCI983045:LCI1048576 LME983045:LME1048576 LWA983045:LWA1048576 MFW983045:MFW1048576 MPS983045:MPS1048576 MZO983045:MZO1048576 NJK983045:NJK1048576 NTG983045:NTG1048576 ODC983045:ODC1048576 OMY983045:OMY1048576 OWU983045:OWU1048576 PGQ983045:PGQ1048576 PQM983045:PQM1048576 QAI983045:QAI1048576 QKE983045:QKE1048576 QUA983045:QUA1048576 RDW983045:RDW1048576 RNS983045:RNS1048576 RXO983045:RXO1048576 SHK983045:SHK1048576 SRG983045:SRG1048576 TBC983045:TBC1048576 TKY983045:TKY1048576 TUU983045:TUU1048576 UEQ983045:UEQ1048576 UOM983045:UOM1048576 UYI983045:UYI1048576 VIE983045:VIE1048576 VSA983045:VSA1048576 WBW983045:WBW1048576 WLS983045:WLS1048576 WVO983045:WVO1048576">
+      <formula1>6</formula1>
+      <formula2>6</formula2>
+    </dataValidation>
+    <dataValidation type="whole" imeMode="off" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="请输入数字" prompt="7" sqref="F5:F65536 JB5:JB65536 SX5:SX65536 ACT5:ACT65536 AMP5:AMP65536 AWL5:AWL65536 BGH5:BGH65536 BQD5:BQD65536 BZZ5:BZZ65536 CJV5:CJV65536 CTR5:CTR65536 DDN5:DDN65536 DNJ5:DNJ65536 DXF5:DXF65536 EHB5:EHB65536 EQX5:EQX65536 FAT5:FAT65536 FKP5:FKP65536 FUL5:FUL65536 GEH5:GEH65536 GOD5:GOD65536 GXZ5:GXZ65536 HHV5:HHV65536 HRR5:HRR65536 IBN5:IBN65536 ILJ5:ILJ65536 IVF5:IVF65536 JFB5:JFB65536 JOX5:JOX65536 JYT5:JYT65536 KIP5:KIP65536 KSL5:KSL65536 LCH5:LCH65536 LMD5:LMD65536 LVZ5:LVZ65536 MFV5:MFV65536 MPR5:MPR65536 MZN5:MZN65536 NJJ5:NJJ65536 NTF5:NTF65536 ODB5:ODB65536 OMX5:OMX65536 OWT5:OWT65536 PGP5:PGP65536 PQL5:PQL65536 QAH5:QAH65536 QKD5:QKD65536 QTZ5:QTZ65536 RDV5:RDV65536 RNR5:RNR65536 RXN5:RXN65536 SHJ5:SHJ65536 SRF5:SRF65536 TBB5:TBB65536 TKX5:TKX65536 TUT5:TUT65536 UEP5:UEP65536 UOL5:UOL65536 UYH5:UYH65536 VID5:VID65536 VRZ5:VRZ65536 WBV5:WBV65536 WLR5:WLR65536 WVN5:WVN65536 F65541:F131072 JB65541:JB131072 SX65541:SX131072 ACT65541:ACT131072 AMP65541:AMP131072 AWL65541:AWL131072 BGH65541:BGH131072 BQD65541:BQD131072 BZZ65541:BZZ131072 CJV65541:CJV131072 CTR65541:CTR131072 DDN65541:DDN131072 DNJ65541:DNJ131072 DXF65541:DXF131072 EHB65541:EHB131072 EQX65541:EQX131072 FAT65541:FAT131072 FKP65541:FKP131072 FUL65541:FUL131072 GEH65541:GEH131072 GOD65541:GOD131072 GXZ65541:GXZ131072 HHV65541:HHV131072 HRR65541:HRR131072 IBN65541:IBN131072 ILJ65541:ILJ131072 IVF65541:IVF131072 JFB65541:JFB131072 JOX65541:JOX131072 JYT65541:JYT131072 KIP65541:KIP131072 KSL65541:KSL131072 LCH65541:LCH131072 LMD65541:LMD131072 LVZ65541:LVZ131072 MFV65541:MFV131072 MPR65541:MPR131072 MZN65541:MZN131072 NJJ65541:NJJ131072 NTF65541:NTF131072 ODB65541:ODB131072 OMX65541:OMX131072 OWT65541:OWT131072 PGP65541:PGP131072 PQL65541:PQL131072 QAH65541:QAH131072 QKD65541:QKD131072 QTZ65541:QTZ131072 RDV65541:RDV131072 RNR65541:RNR131072 RXN65541:RXN131072 SHJ65541:SHJ131072 SRF65541:SRF131072 TBB65541:TBB131072 TKX65541:TKX131072 TUT65541:TUT131072 UEP65541:UEP131072 UOL65541:UOL131072 UYH65541:UYH131072 VID65541:VID131072 VRZ65541:VRZ131072 WBV65541:WBV131072 WLR65541:WLR131072 WVN65541:WVN131072 F131077:F196608 JB131077:JB196608 SX131077:SX196608 ACT131077:ACT196608 AMP131077:AMP196608 AWL131077:AWL196608 BGH131077:BGH196608 BQD131077:BQD196608 BZZ131077:BZZ196608 CJV131077:CJV196608 CTR131077:CTR196608 DDN131077:DDN196608 DNJ131077:DNJ196608 DXF131077:DXF196608 EHB131077:EHB196608 EQX131077:EQX196608 FAT131077:FAT196608 FKP131077:FKP196608 FUL131077:FUL196608 GEH131077:GEH196608 GOD131077:GOD196608 GXZ131077:GXZ196608 HHV131077:HHV196608 HRR131077:HRR196608 IBN131077:IBN196608 ILJ131077:ILJ196608 IVF131077:IVF196608 JFB131077:JFB196608 JOX131077:JOX196608 JYT131077:JYT196608 KIP131077:KIP196608 KSL131077:KSL196608 LCH131077:LCH196608 LMD131077:LMD196608 LVZ131077:LVZ196608 MFV131077:MFV196608 MPR131077:MPR196608 MZN131077:MZN196608 NJJ131077:NJJ196608 NTF131077:NTF196608 ODB131077:ODB196608 OMX131077:OMX196608 OWT131077:OWT196608 PGP131077:PGP196608 PQL131077:PQL196608 QAH131077:QAH196608 QKD131077:QKD196608 QTZ131077:QTZ196608 RDV131077:RDV196608 RNR131077:RNR196608 RXN131077:RXN196608 SHJ131077:SHJ196608 SRF131077:SRF196608 TBB131077:TBB196608 TKX131077:TKX196608 TUT131077:TUT196608 UEP131077:UEP196608 UOL131077:UOL196608 UYH131077:UYH196608 VID131077:VID196608 VRZ131077:VRZ196608 WBV131077:WBV196608 WLR131077:WLR196608 WVN131077:WVN196608 F196613:F262144 JB196613:JB262144 SX196613:SX262144 ACT196613:ACT262144 AMP196613:AMP262144 AWL196613:AWL262144 BGH196613:BGH262144 BQD196613:BQD262144 BZZ196613:BZZ262144 CJV196613:CJV262144 CTR196613:CTR262144 DDN196613:DDN262144 DNJ196613:DNJ262144 DXF196613:DXF262144 EHB196613:EHB262144 EQX196613:EQX262144 FAT196613:FAT262144 FKP196613:FKP262144 FUL196613:FUL262144 GEH196613:GEH262144 GOD196613:GOD262144 GXZ196613:GXZ262144 HHV196613:HHV262144 HRR196613:HRR262144 IBN196613:IBN262144 ILJ196613:ILJ262144 IVF196613:IVF262144 JFB196613:JFB262144 JOX196613:JOX262144 JYT196613:JYT262144 KIP196613:KIP262144 KSL196613:KSL262144 LCH196613:LCH262144 LMD196613:LMD262144 LVZ196613:LVZ262144 MFV196613:MFV262144 MPR196613:MPR262144 MZN196613:MZN262144 NJJ196613:NJJ262144 NTF196613:NTF262144 ODB196613:ODB262144 OMX196613:OMX262144 OWT196613:OWT262144 PGP196613:PGP262144 PQL196613:PQL262144 QAH196613:QAH262144 QKD196613:QKD262144 QTZ196613:QTZ262144 RDV196613:RDV262144 RNR196613:RNR262144 RXN196613:RXN262144 SHJ196613:SHJ262144 SRF196613:SRF262144 TBB196613:TBB262144 TKX196613:TKX262144 TUT196613:TUT262144 UEP196613:UEP262144 UOL196613:UOL262144 UYH196613:UYH262144 VID196613:VID262144 VRZ196613:VRZ262144 WBV196613:WBV262144 WLR196613:WLR262144 WVN196613:WVN262144 F262149:F327680 JB262149:JB327680 SX262149:SX327680 ACT262149:ACT327680 AMP262149:AMP327680 AWL262149:AWL327680 BGH262149:BGH327680 BQD262149:BQD327680 BZZ262149:BZZ327680 CJV262149:CJV327680 CTR262149:CTR327680 DDN262149:DDN327680 DNJ262149:DNJ327680 DXF262149:DXF327680 EHB262149:EHB327680 EQX262149:EQX327680 FAT262149:FAT327680 FKP262149:FKP327680 FUL262149:FUL327680 GEH262149:GEH327680 GOD262149:GOD327680 GXZ262149:GXZ327680 HHV262149:HHV327680 HRR262149:HRR327680 IBN262149:IBN327680 ILJ262149:ILJ327680 IVF262149:IVF327680 JFB262149:JFB327680 JOX262149:JOX327680 JYT262149:JYT327680 KIP262149:KIP327680 KSL262149:KSL327680 LCH262149:LCH327680 LMD262149:LMD327680 LVZ262149:LVZ327680 MFV262149:MFV327680 MPR262149:MPR327680 MZN262149:MZN327680 NJJ262149:NJJ327680 NTF262149:NTF327680 ODB262149:ODB327680 OMX262149:OMX327680 OWT262149:OWT327680 PGP262149:PGP327680 PQL262149:PQL327680 QAH262149:QAH327680 QKD262149:QKD327680 QTZ262149:QTZ327680 RDV262149:RDV327680 RNR262149:RNR327680 RXN262149:RXN327680 SHJ262149:SHJ327680 SRF262149:SRF327680 TBB262149:TBB327680 TKX262149:TKX327680 TUT262149:TUT327680 UEP262149:UEP327680 UOL262149:UOL327680 UYH262149:UYH327680 VID262149:VID327680 VRZ262149:VRZ327680 WBV262149:WBV327680 WLR262149:WLR327680 WVN262149:WVN327680 F327685:F393216 JB327685:JB393216 SX327685:SX393216 ACT327685:ACT393216 AMP327685:AMP393216 AWL327685:AWL393216 BGH327685:BGH393216 BQD327685:BQD393216 BZZ327685:BZZ393216 CJV327685:CJV393216 CTR327685:CTR393216 DDN327685:DDN393216 DNJ327685:DNJ393216 DXF327685:DXF393216 EHB327685:EHB393216 EQX327685:EQX393216 FAT327685:FAT393216 FKP327685:FKP393216 FUL327685:FUL393216 GEH327685:GEH393216 GOD327685:GOD393216 GXZ327685:GXZ393216 HHV327685:HHV393216 HRR327685:HRR393216 IBN327685:IBN393216 ILJ327685:ILJ393216 IVF327685:IVF393216 JFB327685:JFB393216 JOX327685:JOX393216 JYT327685:JYT393216 KIP327685:KIP393216 KSL327685:KSL393216 LCH327685:LCH393216 LMD327685:LMD393216 LVZ327685:LVZ393216 MFV327685:MFV393216 MPR327685:MPR393216 MZN327685:MZN393216 NJJ327685:NJJ393216 NTF327685:NTF393216 ODB327685:ODB393216 OMX327685:OMX393216 OWT327685:OWT393216 PGP327685:PGP393216 PQL327685:PQL393216 QAH327685:QAH393216 QKD327685:QKD393216 QTZ327685:QTZ393216 RDV327685:RDV393216 RNR327685:RNR393216 RXN327685:RXN393216 SHJ327685:SHJ393216 SRF327685:SRF393216 TBB327685:TBB393216 TKX327685:TKX393216 TUT327685:TUT393216 UEP327685:UEP393216 UOL327685:UOL393216 UYH327685:UYH393216 VID327685:VID393216 VRZ327685:VRZ393216 WBV327685:WBV393216 WLR327685:WLR393216 WVN327685:WVN393216 F393221:F458752 JB393221:JB458752 SX393221:SX458752 ACT393221:ACT458752 AMP393221:AMP458752 AWL393221:AWL458752 BGH393221:BGH458752 BQD393221:BQD458752 BZZ393221:BZZ458752 CJV393221:CJV458752 CTR393221:CTR458752 DDN393221:DDN458752 DNJ393221:DNJ458752 DXF393221:DXF458752 EHB393221:EHB458752 EQX393221:EQX458752 FAT393221:FAT458752 FKP393221:FKP458752 FUL393221:FUL458752 GEH393221:GEH458752 GOD393221:GOD458752 GXZ393221:GXZ458752 HHV393221:HHV458752 HRR393221:HRR458752 IBN393221:IBN458752 ILJ393221:ILJ458752 IVF393221:IVF458752 JFB393221:JFB458752 JOX393221:JOX458752 JYT393221:JYT458752 KIP393221:KIP458752 KSL393221:KSL458752 LCH393221:LCH458752 LMD393221:LMD458752 LVZ393221:LVZ458752 MFV393221:MFV458752 MPR393221:MPR458752 MZN393221:MZN458752 NJJ393221:NJJ458752 NTF393221:NTF458752 ODB393221:ODB458752 OMX393221:OMX458752 OWT393221:OWT458752 PGP393221:PGP458752 PQL393221:PQL458752 QAH393221:QAH458752 QKD393221:QKD458752 QTZ393221:QTZ458752 RDV393221:RDV458752 RNR393221:RNR458752 RXN393221:RXN458752 SHJ393221:SHJ458752 SRF393221:SRF458752 TBB393221:TBB458752 TKX393221:TKX458752 TUT393221:TUT458752 UEP393221:UEP458752 UOL393221:UOL458752 UYH393221:UYH458752 VID393221:VID458752 VRZ393221:VRZ458752 WBV393221:WBV458752 WLR393221:WLR458752 WVN393221:WVN458752 F458757:F524288 JB458757:JB524288 SX458757:SX524288 ACT458757:ACT524288 AMP458757:AMP524288 AWL458757:AWL524288 BGH458757:BGH524288 BQD458757:BQD524288 BZZ458757:BZZ524288 CJV458757:CJV524288 CTR458757:CTR524288 DDN458757:DDN524288 DNJ458757:DNJ524288 DXF458757:DXF524288 EHB458757:EHB524288 EQX458757:EQX524288 FAT458757:FAT524288 FKP458757:FKP524288 FUL458757:FUL524288 GEH458757:GEH524288 GOD458757:GOD524288 GXZ458757:GXZ524288 HHV458757:HHV524288 HRR458757:HRR524288 IBN458757:IBN524288 ILJ458757:ILJ524288 IVF458757:IVF524288 JFB458757:JFB524288 JOX458757:JOX524288 JYT458757:JYT524288 KIP458757:KIP524288 KSL458757:KSL524288 LCH458757:LCH524288 LMD458757:LMD524288 LVZ458757:LVZ524288 MFV458757:MFV524288 MPR458757:MPR524288 MZN458757:MZN524288 NJJ458757:NJJ524288 NTF458757:NTF524288 ODB458757:ODB524288 OMX458757:OMX524288 OWT458757:OWT524288 PGP458757:PGP524288 PQL458757:PQL524288 QAH458757:QAH524288 QKD458757:QKD524288 QTZ458757:QTZ524288 RDV458757:RDV524288 RNR458757:RNR524288 RXN458757:RXN524288 SHJ458757:SHJ524288 SRF458757:SRF524288 TBB458757:TBB524288 TKX458757:TKX524288 TUT458757:TUT524288 UEP458757:UEP524288 UOL458757:UOL524288 UYH458757:UYH524288 VID458757:VID524288 VRZ458757:VRZ524288 WBV458757:WBV524288 WLR458757:WLR524288 WVN458757:WVN524288 F524293:F589824 JB524293:JB589824 SX524293:SX589824 ACT524293:ACT589824 AMP524293:AMP589824 AWL524293:AWL589824 BGH524293:BGH589824 BQD524293:BQD589824 BZZ524293:BZZ589824 CJV524293:CJV589824 CTR524293:CTR589824 DDN524293:DDN589824 DNJ524293:DNJ589824 DXF524293:DXF589824 EHB524293:EHB589824 EQX524293:EQX589824 FAT524293:FAT589824 FKP524293:FKP589824 FUL524293:FUL589824 GEH524293:GEH589824 GOD524293:GOD589824 GXZ524293:GXZ589824 HHV524293:HHV589824 HRR524293:HRR589824 IBN524293:IBN589824 ILJ524293:ILJ589824 IVF524293:IVF589824 JFB524293:JFB589824 JOX524293:JOX589824 JYT524293:JYT589824 KIP524293:KIP589824 KSL524293:KSL589824 LCH524293:LCH589824 LMD524293:LMD589824 LVZ524293:LVZ589824 MFV524293:MFV589824 MPR524293:MPR589824 MZN524293:MZN589824 NJJ524293:NJJ589824 NTF524293:NTF589824 ODB524293:ODB589824 OMX524293:OMX589824 OWT524293:OWT589824 PGP524293:PGP589824 PQL524293:PQL589824 QAH524293:QAH589824 QKD524293:QKD589824 QTZ524293:QTZ589824 RDV524293:RDV589824 RNR524293:RNR589824 RXN524293:RXN589824 SHJ524293:SHJ589824 SRF524293:SRF589824 TBB524293:TBB589824 TKX524293:TKX589824 TUT524293:TUT589824 UEP524293:UEP589824 UOL524293:UOL589824 UYH524293:UYH589824 VID524293:VID589824 VRZ524293:VRZ589824 WBV524293:WBV589824 WLR524293:WLR589824 WVN524293:WVN589824 F589829:F655360 JB589829:JB655360 SX589829:SX655360 ACT589829:ACT655360 AMP589829:AMP655360 AWL589829:AWL655360 BGH589829:BGH655360 BQD589829:BQD655360 BZZ589829:BZZ655360 CJV589829:CJV655360 CTR589829:CTR655360 DDN589829:DDN655360 DNJ589829:DNJ655360 DXF589829:DXF655360 EHB589829:EHB655360 EQX589829:EQX655360 FAT589829:FAT655360 FKP589829:FKP655360 FUL589829:FUL655360 GEH589829:GEH655360 GOD589829:GOD655360 GXZ589829:GXZ655360 HHV589829:HHV655360 HRR589829:HRR655360 IBN589829:IBN655360 ILJ589829:ILJ655360 IVF589829:IVF655360 JFB589829:JFB655360 JOX589829:JOX655360 JYT589829:JYT655360 KIP589829:KIP655360 KSL589829:KSL655360 LCH589829:LCH655360 LMD589829:LMD655360 LVZ589829:LVZ655360 MFV589829:MFV655360 MPR589829:MPR655360 MZN589829:MZN655360 NJJ589829:NJJ655360 NTF589829:NTF655360 ODB589829:ODB655360 OMX589829:OMX655360 OWT589829:OWT655360 PGP589829:PGP655360 PQL589829:PQL655360 QAH589829:QAH655360 QKD589829:QKD655360 QTZ589829:QTZ655360 RDV589829:RDV655360 RNR589829:RNR655360 RXN589829:RXN655360 SHJ589829:SHJ655360 SRF589829:SRF655360 TBB589829:TBB655360 TKX589829:TKX655360 TUT589829:TUT655360 UEP589829:UEP655360 UOL589829:UOL655360 UYH589829:UYH655360 VID589829:VID655360 VRZ589829:VRZ655360 WBV589829:WBV655360 WLR589829:WLR655360 WVN589829:WVN655360 F655365:F720896 JB655365:JB720896 SX655365:SX720896 ACT655365:ACT720896 AMP655365:AMP720896 AWL655365:AWL720896 BGH655365:BGH720896 BQD655365:BQD720896 BZZ655365:BZZ720896 CJV655365:CJV720896 CTR655365:CTR720896 DDN655365:DDN720896 DNJ655365:DNJ720896 DXF655365:DXF720896 EHB655365:EHB720896 EQX655365:EQX720896 FAT655365:FAT720896 FKP655365:FKP720896 FUL655365:FUL720896 GEH655365:GEH720896 GOD655365:GOD720896 GXZ655365:GXZ720896 HHV655365:HHV720896 HRR655365:HRR720896 IBN655365:IBN720896 ILJ655365:ILJ720896 IVF655365:IVF720896 JFB655365:JFB720896 JOX655365:JOX720896 JYT655365:JYT720896 KIP655365:KIP720896 KSL655365:KSL720896 LCH655365:LCH720896 LMD655365:LMD720896 LVZ655365:LVZ720896 MFV655365:MFV720896 MPR655365:MPR720896 MZN655365:MZN720896 NJJ655365:NJJ720896 NTF655365:NTF720896 ODB655365:ODB720896 OMX655365:OMX720896 OWT655365:OWT720896 PGP655365:PGP720896 PQL655365:PQL720896 QAH655365:QAH720896 QKD655365:QKD720896 QTZ655365:QTZ720896 RDV655365:RDV720896 RNR655365:RNR720896 RXN655365:RXN720896 SHJ655365:SHJ720896 SRF655365:SRF720896 TBB655365:TBB720896 TKX655365:TKX720896 TUT655365:TUT720896 UEP655365:UEP720896 UOL655365:UOL720896 UYH655365:UYH720896 VID655365:VID720896 VRZ655365:VRZ720896 WBV655365:WBV720896 WLR655365:WLR720896 WVN655365:WVN720896 F720901:F786432 JB720901:JB786432 SX720901:SX786432 ACT720901:ACT786432 AMP720901:AMP786432 AWL720901:AWL786432 BGH720901:BGH786432 BQD720901:BQD786432 BZZ720901:BZZ786432 CJV720901:CJV786432 CTR720901:CTR786432 DDN720901:DDN786432 DNJ720901:DNJ786432 DXF720901:DXF786432 EHB720901:EHB786432 EQX720901:EQX786432 FAT720901:FAT786432 FKP720901:FKP786432 FUL720901:FUL786432 GEH720901:GEH786432 GOD720901:GOD786432 GXZ720901:GXZ786432 HHV720901:HHV786432 HRR720901:HRR786432 IBN720901:IBN786432 ILJ720901:ILJ786432 IVF720901:IVF786432 JFB720901:JFB786432 JOX720901:JOX786432 JYT720901:JYT786432 KIP720901:KIP786432 KSL720901:KSL786432 LCH720901:LCH786432 LMD720901:LMD786432 LVZ720901:LVZ786432 MFV720901:MFV786432 MPR720901:MPR786432 MZN720901:MZN786432 NJJ720901:NJJ786432 NTF720901:NTF786432 ODB720901:ODB786432 OMX720901:OMX786432 OWT720901:OWT786432 PGP720901:PGP786432 PQL720901:PQL786432 QAH720901:QAH786432 QKD720901:QKD786432 QTZ720901:QTZ786432 RDV720901:RDV786432 RNR720901:RNR786432 RXN720901:RXN786432 SHJ720901:SHJ786432 SRF720901:SRF786432 TBB720901:TBB786432 TKX720901:TKX786432 TUT720901:TUT786432 UEP720901:UEP786432 UOL720901:UOL786432 UYH720901:UYH786432 VID720901:VID786432 VRZ720901:VRZ786432 WBV720901:WBV786432 WLR720901:WLR786432 WVN720901:WVN786432 F786437:F851968 JB786437:JB851968 SX786437:SX851968 ACT786437:ACT851968 AMP786437:AMP851968 AWL786437:AWL851968 BGH786437:BGH851968 BQD786437:BQD851968 BZZ786437:BZZ851968 CJV786437:CJV851968 CTR786437:CTR851968 DDN786437:DDN851968 DNJ786437:DNJ851968 DXF786437:DXF851968 EHB786437:EHB851968 EQX786437:EQX851968 FAT786437:FAT851968 FKP786437:FKP851968 FUL786437:FUL851968 GEH786437:GEH851968 GOD786437:GOD851968 GXZ786437:GXZ851968 HHV786437:HHV851968 HRR786437:HRR851968 IBN786437:IBN851968 ILJ786437:ILJ851968 IVF786437:IVF851968 JFB786437:JFB851968 JOX786437:JOX851968 JYT786437:JYT851968 KIP786437:KIP851968 KSL786437:KSL851968 LCH786437:LCH851968 LMD786437:LMD851968 LVZ786437:LVZ851968 MFV786437:MFV851968 MPR786437:MPR851968 MZN786437:MZN851968 NJJ786437:NJJ851968 NTF786437:NTF851968 ODB786437:ODB851968 OMX786437:OMX851968 OWT786437:OWT851968 PGP786437:PGP851968 PQL786437:PQL851968 QAH786437:QAH851968 QKD786437:QKD851968 QTZ786437:QTZ851968 RDV786437:RDV851968 RNR786437:RNR851968 RXN786437:RXN851968 SHJ786437:SHJ851968 SRF786437:SRF851968 TBB786437:TBB851968 TKX786437:TKX851968 TUT786437:TUT851968 UEP786437:UEP851968 UOL786437:UOL851968 UYH786437:UYH851968 VID786437:VID851968 VRZ786437:VRZ851968 WBV786437:WBV851968 WLR786437:WLR851968 WVN786437:WVN851968 F851973:F917504 JB851973:JB917504 SX851973:SX917504 ACT851973:ACT917504 AMP851973:AMP917504 AWL851973:AWL917504 BGH851973:BGH917504 BQD851973:BQD917504 BZZ851973:BZZ917504 CJV851973:CJV917504 CTR851973:CTR917504 DDN851973:DDN917504 DNJ851973:DNJ917504 DXF851973:DXF917504 EHB851973:EHB917504 EQX851973:EQX917504 FAT851973:FAT917504 FKP851973:FKP917504 FUL851973:FUL917504 GEH851973:GEH917504 GOD851973:GOD917504 GXZ851973:GXZ917504 HHV851973:HHV917504 HRR851973:HRR917504 IBN851973:IBN917504 ILJ851973:ILJ917504 IVF851973:IVF917504 JFB851973:JFB917504 JOX851973:JOX917504 JYT851973:JYT917504 KIP851973:KIP917504 KSL851973:KSL917504 LCH851973:LCH917504 LMD851973:LMD917504 LVZ851973:LVZ917504 MFV851973:MFV917504 MPR851973:MPR917504 MZN851973:MZN917504 NJJ851973:NJJ917504 NTF851973:NTF917504 ODB851973:ODB917504 OMX851973:OMX917504 OWT851973:OWT917504 PGP851973:PGP917504 PQL851973:PQL917504 QAH851973:QAH917504 QKD851973:QKD917504 QTZ851973:QTZ917504 RDV851973:RDV917504 RNR851973:RNR917504 RXN851973:RXN917504 SHJ851973:SHJ917504 SRF851973:SRF917504 TBB851973:TBB917504 TKX851973:TKX917504 TUT851973:TUT917504 UEP851973:UEP917504 UOL851973:UOL917504 UYH851973:UYH917504 VID851973:VID917504 VRZ851973:VRZ917504 WBV851973:WBV917504 WLR851973:WLR917504 WVN851973:WVN917504 F917509:F983040 JB917509:JB983040 SX917509:SX983040 ACT917509:ACT983040 AMP917509:AMP983040 AWL917509:AWL983040 BGH917509:BGH983040 BQD917509:BQD983040 BZZ917509:BZZ983040 CJV917509:CJV983040 CTR917509:CTR983040 DDN917509:DDN983040 DNJ917509:DNJ983040 DXF917509:DXF983040 EHB917509:EHB983040 EQX917509:EQX983040 FAT917509:FAT983040 FKP917509:FKP983040 FUL917509:FUL983040 GEH917509:GEH983040 GOD917509:GOD983040 GXZ917509:GXZ983040 HHV917509:HHV983040 HRR917509:HRR983040 IBN917509:IBN983040 ILJ917509:ILJ983040 IVF917509:IVF983040 JFB917509:JFB983040 JOX917509:JOX983040 JYT917509:JYT983040 KIP917509:KIP983040 KSL917509:KSL983040 LCH917509:LCH983040 LMD917509:LMD983040 LVZ917509:LVZ983040 MFV917509:MFV983040 MPR917509:MPR983040 MZN917509:MZN983040 NJJ917509:NJJ983040 NTF917509:NTF983040 ODB917509:ODB983040 OMX917509:OMX983040 OWT917509:OWT983040 PGP917509:PGP983040 PQL917509:PQL983040 QAH917509:QAH983040 QKD917509:QKD983040 QTZ917509:QTZ983040 RDV917509:RDV983040 RNR917509:RNR983040 RXN917509:RXN983040 SHJ917509:SHJ983040 SRF917509:SRF983040 TBB917509:TBB983040 TKX917509:TKX983040 TUT917509:TUT983040 UEP917509:UEP983040 UOL917509:UOL983040 UYH917509:UYH983040 VID917509:VID983040 VRZ917509:VRZ983040 WBV917509:WBV983040 WLR917509:WLR983040 WVN917509:WVN983040 F983045:F1048576 JB983045:JB1048576 SX983045:SX1048576 ACT983045:ACT1048576 AMP983045:AMP1048576 AWL983045:AWL1048576 BGH983045:BGH1048576 BQD983045:BQD1048576 BZZ983045:BZZ1048576 CJV983045:CJV1048576 CTR983045:CTR1048576 DDN983045:DDN1048576 DNJ983045:DNJ1048576 DXF983045:DXF1048576 EHB983045:EHB1048576 EQX983045:EQX1048576 FAT983045:FAT1048576 FKP983045:FKP1048576 FUL983045:FUL1048576 GEH983045:GEH1048576 GOD983045:GOD1048576 GXZ983045:GXZ1048576 HHV983045:HHV1048576 HRR983045:HRR1048576 IBN983045:IBN1048576 ILJ983045:ILJ1048576 IVF983045:IVF1048576 JFB983045:JFB1048576 JOX983045:JOX1048576 JYT983045:JYT1048576 KIP983045:KIP1048576 KSL983045:KSL1048576 LCH983045:LCH1048576 LMD983045:LMD1048576 LVZ983045:LVZ1048576 MFV983045:MFV1048576 MPR983045:MPR1048576 MZN983045:MZN1048576 NJJ983045:NJJ1048576 NTF983045:NTF1048576 ODB983045:ODB1048576 OMX983045:OMX1048576 OWT983045:OWT1048576 PGP983045:PGP1048576 PQL983045:PQL1048576 QAH983045:QAH1048576 QKD983045:QKD1048576 QTZ983045:QTZ1048576 RDV983045:RDV1048576 RNR983045:RNR1048576 RXN983045:RXN1048576 SHJ983045:SHJ1048576 SRF983045:SRF1048576 TBB983045:TBB1048576 TKX983045:TKX1048576 TUT983045:TUT1048576 UEP983045:UEP1048576 UOL983045:UOL1048576 UYH983045:UYH1048576 VID983045:VID1048576 VRZ983045:VRZ1048576 WBV983045:WBV1048576 WLR983045:WLR1048576 WVN983045:WVN1048576">
+      <formula1>7</formula1>
+      <formula2>7</formula2>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A5:A65536 IW5:IW65536 SS5:SS65536 ACO5:ACO65536 AMK5:AMK65536 AWG5:AWG65536 BGC5:BGC65536 BPY5:BPY65536 BZU5:BZU65536 CJQ5:CJQ65536 CTM5:CTM65536 DDI5:DDI65536 DNE5:DNE65536 DXA5:DXA65536 EGW5:EGW65536 EQS5:EQS65536 FAO5:FAO65536 FKK5:FKK65536 FUG5:FUG65536 GEC5:GEC65536 GNY5:GNY65536 GXU5:GXU65536 HHQ5:HHQ65536 HRM5:HRM65536 IBI5:IBI65536 ILE5:ILE65536 IVA5:IVA65536 JEW5:JEW65536 JOS5:JOS65536 JYO5:JYO65536 KIK5:KIK65536 KSG5:KSG65536 LCC5:LCC65536 LLY5:LLY65536 LVU5:LVU65536 MFQ5:MFQ65536 MPM5:MPM65536 MZI5:MZI65536 NJE5:NJE65536 NTA5:NTA65536 OCW5:OCW65536 OMS5:OMS65536 OWO5:OWO65536 PGK5:PGK65536 PQG5:PQG65536 QAC5:QAC65536 QJY5:QJY65536 QTU5:QTU65536 RDQ5:RDQ65536 RNM5:RNM65536 RXI5:RXI65536 SHE5:SHE65536 SRA5:SRA65536 TAW5:TAW65536 TKS5:TKS65536 TUO5:TUO65536 UEK5:UEK65536 UOG5:UOG65536 UYC5:UYC65536 VHY5:VHY65536 VRU5:VRU65536 WBQ5:WBQ65536 WLM5:WLM65536 WVI5:WVI65536 A65541:A131072 IW65541:IW131072 SS65541:SS131072 ACO65541:ACO131072 AMK65541:AMK131072 AWG65541:AWG131072 BGC65541:BGC131072 BPY65541:BPY131072 BZU65541:BZU131072 CJQ65541:CJQ131072 CTM65541:CTM131072 DDI65541:DDI131072 DNE65541:DNE131072 DXA65541:DXA131072 EGW65541:EGW131072 EQS65541:EQS131072 FAO65541:FAO131072 FKK65541:FKK131072 FUG65541:FUG131072 GEC65541:GEC131072 GNY65541:GNY131072 GXU65541:GXU131072 HHQ65541:HHQ131072 HRM65541:HRM131072 IBI65541:IBI131072 ILE65541:ILE131072 IVA65541:IVA131072 JEW65541:JEW131072 JOS65541:JOS131072 JYO65541:JYO131072 KIK65541:KIK131072 KSG65541:KSG131072 LCC65541:LCC131072 LLY65541:LLY131072 LVU65541:LVU131072 MFQ65541:MFQ131072 MPM65541:MPM131072 MZI65541:MZI131072 NJE65541:NJE131072 NTA65541:NTA131072 OCW65541:OCW131072 OMS65541:OMS131072 OWO65541:OWO131072 PGK65541:PGK131072 PQG65541:PQG131072 QAC65541:QAC131072 QJY65541:QJY131072 QTU65541:QTU131072 RDQ65541:RDQ131072 RNM65541:RNM131072 RXI65541:RXI131072 SHE65541:SHE131072 SRA65541:SRA131072 TAW65541:TAW131072 TKS65541:TKS131072 TUO65541:TUO131072 UEK65541:UEK131072 UOG65541:UOG131072 UYC65541:UYC131072 VHY65541:VHY131072 VRU65541:VRU131072 WBQ65541:WBQ131072 WLM65541:WLM131072 WVI65541:WVI131072 A131077:A196608 IW131077:IW196608 SS131077:SS196608 ACO131077:ACO196608 AMK131077:AMK196608 AWG131077:AWG196608 BGC131077:BGC196608 BPY131077:BPY196608 BZU131077:BZU196608 CJQ131077:CJQ196608 CTM131077:CTM196608 DDI131077:DDI196608 DNE131077:DNE196608 DXA131077:DXA196608 EGW131077:EGW196608 EQS131077:EQS196608 FAO131077:FAO196608 FKK131077:FKK196608 FUG131077:FUG196608 GEC131077:GEC196608 GNY131077:GNY196608 GXU131077:GXU196608 HHQ131077:HHQ196608 HRM131077:HRM196608 IBI131077:IBI196608 ILE131077:ILE196608 IVA131077:IVA196608 JEW131077:JEW196608 JOS131077:JOS196608 JYO131077:JYO196608 KIK131077:KIK196608 KSG131077:KSG196608 LCC131077:LCC196608 LLY131077:LLY196608 LVU131077:LVU196608 MFQ131077:MFQ196608 MPM131077:MPM196608 MZI131077:MZI196608 NJE131077:NJE196608 NTA131077:NTA196608 OCW131077:OCW196608 OMS131077:OMS196608 OWO131077:OWO196608 PGK131077:PGK196608 PQG131077:PQG196608 QAC131077:QAC196608 QJY131077:QJY196608 QTU131077:QTU196608 RDQ131077:RDQ196608 RNM131077:RNM196608 RXI131077:RXI196608 SHE131077:SHE196608 SRA131077:SRA196608 TAW131077:TAW196608 TKS131077:TKS196608 TUO131077:TUO196608 UEK131077:UEK196608 UOG131077:UOG196608 UYC131077:UYC196608 VHY131077:VHY196608 VRU131077:VRU196608 WBQ131077:WBQ196608 WLM131077:WLM196608 WVI131077:WVI196608 A196613:A262144 IW196613:IW262144 SS196613:SS262144 ACO196613:ACO262144 AMK196613:AMK262144 AWG196613:AWG262144 BGC196613:BGC262144 BPY196613:BPY262144 BZU196613:BZU262144 CJQ196613:CJQ262144 CTM196613:CTM262144 DDI196613:DDI262144 DNE196613:DNE262144 DXA196613:DXA262144 EGW196613:EGW262144 EQS196613:EQS262144 FAO196613:FAO262144 FKK196613:FKK262144 FUG196613:FUG262144 GEC196613:GEC262144 GNY196613:GNY262144 GXU196613:GXU262144 HHQ196613:HHQ262144 HRM196613:HRM262144 IBI196613:IBI262144 ILE196613:ILE262144 IVA196613:IVA262144 JEW196613:JEW262144 JOS196613:JOS262144 JYO196613:JYO262144 KIK196613:KIK262144 KSG196613:KSG262144 LCC196613:LCC262144 LLY196613:LLY262144 LVU196613:LVU262144 MFQ196613:MFQ262144 MPM196613:MPM262144 MZI196613:MZI262144 NJE196613:NJE262144 NTA196613:NTA262144 OCW196613:OCW262144 OMS196613:OMS262144 OWO196613:OWO262144 PGK196613:PGK262144 PQG196613:PQG262144 QAC196613:QAC262144 QJY196613:QJY262144 QTU196613:QTU262144 RDQ196613:RDQ262144 RNM196613:RNM262144 RXI196613:RXI262144 SHE196613:SHE262144 SRA196613:SRA262144 TAW196613:TAW262144 TKS196613:TKS262144 TUO196613:TUO262144 UEK196613:UEK262144 UOG196613:UOG262144 UYC196613:UYC262144 VHY196613:VHY262144 VRU196613:VRU262144 WBQ196613:WBQ262144 WLM196613:WLM262144 WVI196613:WVI262144 A262149:A327680 IW262149:IW327680 SS262149:SS327680 ACO262149:ACO327680 AMK262149:AMK327680 AWG262149:AWG327680 BGC262149:BGC327680 BPY262149:BPY327680 BZU262149:BZU327680 CJQ262149:CJQ327680 CTM262149:CTM327680 DDI262149:DDI327680 DNE262149:DNE327680 DXA262149:DXA327680 EGW262149:EGW327680 EQS262149:EQS327680 FAO262149:FAO327680 FKK262149:FKK327680 FUG262149:FUG327680 GEC262149:GEC327680 GNY262149:GNY327680 GXU262149:GXU327680 HHQ262149:HHQ327680 HRM262149:HRM327680 IBI262149:IBI327680 ILE262149:ILE327680 IVA262149:IVA327680 JEW262149:JEW327680 JOS262149:JOS327680 JYO262149:JYO327680 KIK262149:KIK327680 KSG262149:KSG327680 LCC262149:LCC327680 LLY262149:LLY327680 LVU262149:LVU327680 MFQ262149:MFQ327680 MPM262149:MPM327680 MZI262149:MZI327680 NJE262149:NJE327680 NTA262149:NTA327680 OCW262149:OCW327680 OMS262149:OMS327680 OWO262149:OWO327680 PGK262149:PGK327680 PQG262149:PQG327680 QAC262149:QAC327680 QJY262149:QJY327680 QTU262149:QTU327680 RDQ262149:RDQ327680 RNM262149:RNM327680 RXI262149:RXI327680 SHE262149:SHE327680 SRA262149:SRA327680 TAW262149:TAW327680 TKS262149:TKS327680 TUO262149:TUO327680 UEK262149:UEK327680 UOG262149:UOG327680 UYC262149:UYC327680 VHY262149:VHY327680 VRU262149:VRU327680 WBQ262149:WBQ327680 WLM262149:WLM327680 WVI262149:WVI327680 A327685:A393216 IW327685:IW393216 SS327685:SS393216 ACO327685:ACO393216 AMK327685:AMK393216 AWG327685:AWG393216 BGC327685:BGC393216 BPY327685:BPY393216 BZU327685:BZU393216 CJQ327685:CJQ393216 CTM327685:CTM393216 DDI327685:DDI393216 DNE327685:DNE393216 DXA327685:DXA393216 EGW327685:EGW393216 EQS327685:EQS393216 FAO327685:FAO393216 FKK327685:FKK393216 FUG327685:FUG393216 GEC327685:GEC393216 GNY327685:GNY393216 GXU327685:GXU393216 HHQ327685:HHQ393216 HRM327685:HRM393216 IBI327685:IBI393216 ILE327685:ILE393216 IVA327685:IVA393216 JEW327685:JEW393216 JOS327685:JOS393216 JYO327685:JYO393216 KIK327685:KIK393216 KSG327685:KSG393216 LCC327685:LCC393216 LLY327685:LLY393216 LVU327685:LVU393216 MFQ327685:MFQ393216 MPM327685:MPM393216 MZI327685:MZI393216 NJE327685:NJE393216 NTA327685:NTA393216 OCW327685:OCW393216 OMS327685:OMS393216 OWO327685:OWO393216 PGK327685:PGK393216 PQG327685:PQG393216 QAC327685:QAC393216 QJY327685:QJY393216 QTU327685:QTU393216 RDQ327685:RDQ393216 RNM327685:RNM393216 RXI327685:RXI393216 SHE327685:SHE393216 SRA327685:SRA393216 TAW327685:TAW393216 TKS327685:TKS393216 TUO327685:TUO393216 UEK327685:UEK393216 UOG327685:UOG393216 UYC327685:UYC393216 VHY327685:VHY393216 VRU327685:VRU393216 WBQ327685:WBQ393216 WLM327685:WLM393216 WVI327685:WVI393216 A393221:A458752 IW393221:IW458752 SS393221:SS458752 ACO393221:ACO458752 AMK393221:AMK458752 AWG393221:AWG458752 BGC393221:BGC458752 BPY393221:BPY458752 BZU393221:BZU458752 CJQ393221:CJQ458752 CTM393221:CTM458752 DDI393221:DDI458752 DNE393221:DNE458752 DXA393221:DXA458752 EGW393221:EGW458752 EQS393221:EQS458752 FAO393221:FAO458752 FKK393221:FKK458752 FUG393221:FUG458752 GEC393221:GEC458752 GNY393221:GNY458752 GXU393221:GXU458752 HHQ393221:HHQ458752 HRM393221:HRM458752 IBI393221:IBI458752 ILE393221:ILE458752 IVA393221:IVA458752 JEW393221:JEW458752 JOS393221:JOS458752 JYO393221:JYO458752 KIK393221:KIK458752 KSG393221:KSG458752 LCC393221:LCC458752 LLY393221:LLY458752 LVU393221:LVU458752 MFQ393221:MFQ458752 MPM393221:MPM458752 MZI393221:MZI458752 NJE393221:NJE458752 NTA393221:NTA458752 OCW393221:OCW458752 OMS393221:OMS458752 OWO393221:OWO458752 PGK393221:PGK458752 PQG393221:PQG458752 QAC393221:QAC458752 QJY393221:QJY458752 QTU393221:QTU458752 RDQ393221:RDQ458752 RNM393221:RNM458752 RXI393221:RXI458752 SHE393221:SHE458752 SRA393221:SRA458752 TAW393221:TAW458752 TKS393221:TKS458752 TUO393221:TUO458752 UEK393221:UEK458752 UOG393221:UOG458752 UYC393221:UYC458752 VHY393221:VHY458752 VRU393221:VRU458752 WBQ393221:WBQ458752 WLM393221:WLM458752 WVI393221:WVI458752 A458757:A524288 IW458757:IW524288 SS458757:SS524288 ACO458757:ACO524288 AMK458757:AMK524288 AWG458757:AWG524288 BGC458757:BGC524288 BPY458757:BPY524288 BZU458757:BZU524288 CJQ458757:CJQ524288 CTM458757:CTM524288 DDI458757:DDI524288 DNE458757:DNE524288 DXA458757:DXA524288 EGW458757:EGW524288 EQS458757:EQS524288 FAO458757:FAO524288 FKK458757:FKK524288 FUG458757:FUG524288 GEC458757:GEC524288 GNY458757:GNY524288 GXU458757:GXU524288 HHQ458757:HHQ524288 HRM458757:HRM524288 IBI458757:IBI524288 ILE458757:ILE524288 IVA458757:IVA524288 JEW458757:JEW524288 JOS458757:JOS524288 JYO458757:JYO524288 KIK458757:KIK524288 KSG458757:KSG524288 LCC458757:LCC524288 LLY458757:LLY524288 LVU458757:LVU524288 MFQ458757:MFQ524288 MPM458757:MPM524288 MZI458757:MZI524288 NJE458757:NJE524288 NTA458757:NTA524288 OCW458757:OCW524288 OMS458757:OMS524288 OWO458757:OWO524288 PGK458757:PGK524288 PQG458757:PQG524288 QAC458757:QAC524288 QJY458757:QJY524288 QTU458757:QTU524288 RDQ458757:RDQ524288 RNM458757:RNM524288 RXI458757:RXI524288 SHE458757:SHE524288 SRA458757:SRA524288 TAW458757:TAW524288 TKS458757:TKS524288 TUO458757:TUO524288 UEK458757:UEK524288 UOG458757:UOG524288 UYC458757:UYC524288 VHY458757:VHY524288 VRU458757:VRU524288 WBQ458757:WBQ524288 WLM458757:WLM524288 WVI458757:WVI524288 A524293:A589824 IW524293:IW589824 SS524293:SS589824 ACO524293:ACO589824 AMK524293:AMK589824 AWG524293:AWG589824 BGC524293:BGC589824 BPY524293:BPY589824 BZU524293:BZU589824 CJQ524293:CJQ589824 CTM524293:CTM589824 DDI524293:DDI589824 DNE524293:DNE589824 DXA524293:DXA589824 EGW524293:EGW589824 EQS524293:EQS589824 FAO524293:FAO589824 FKK524293:FKK589824 FUG524293:FUG589824 GEC524293:GEC589824 GNY524293:GNY589824 GXU524293:GXU589824 HHQ524293:HHQ589824 HRM524293:HRM589824 IBI524293:IBI589824 ILE524293:ILE589824 IVA524293:IVA589824 JEW524293:JEW589824 JOS524293:JOS589824 JYO524293:JYO589824 KIK524293:KIK589824 KSG524293:KSG589824 LCC524293:LCC589824 LLY524293:LLY589824 LVU524293:LVU589824 MFQ524293:MFQ589824 MPM524293:MPM589824 MZI524293:MZI589824 NJE524293:NJE589824 NTA524293:NTA589824 OCW524293:OCW589824 OMS524293:OMS589824 OWO524293:OWO589824 PGK524293:PGK589824 PQG524293:PQG589824 QAC524293:QAC589824 QJY524293:QJY589824 QTU524293:QTU589824 RDQ524293:RDQ589824 RNM524293:RNM589824 RXI524293:RXI589824 SHE524293:SHE589824 SRA524293:SRA589824 TAW524293:TAW589824 TKS524293:TKS589824 TUO524293:TUO589824 UEK524293:UEK589824 UOG524293:UOG589824 UYC524293:UYC589824 VHY524293:VHY589824 VRU524293:VRU589824 WBQ524293:WBQ589824 WLM524293:WLM589824 WVI524293:WVI589824 A589829:A655360 IW589829:IW655360 SS589829:SS655360 ACO589829:ACO655360 AMK589829:AMK655360 AWG589829:AWG655360 BGC589829:BGC655360 BPY589829:BPY655360 BZU589829:BZU655360 CJQ589829:CJQ655360 CTM589829:CTM655360 DDI589829:DDI655360 DNE589829:DNE655360 DXA589829:DXA655360 EGW589829:EGW655360 EQS589829:EQS655360 FAO589829:FAO655360 FKK589829:FKK655360 FUG589829:FUG655360 GEC589829:GEC655360 GNY589829:GNY655360 GXU589829:GXU655360 HHQ589829:HHQ655360 HRM589829:HRM655360 IBI589829:IBI655360 ILE589829:ILE655360 IVA589829:IVA655360 JEW589829:JEW655360 JOS589829:JOS655360 JYO589829:JYO655360 KIK589829:KIK655360 KSG589829:KSG655360 LCC589829:LCC655360 LLY589829:LLY655360 LVU589829:LVU655360 MFQ589829:MFQ655360 MPM589829:MPM655360 MZI589829:MZI655360 NJE589829:NJE655360 NTA589829:NTA655360 OCW589829:OCW655360 OMS589829:OMS655360 OWO589829:OWO655360 PGK589829:PGK655360 PQG589829:PQG655360 QAC589829:QAC655360 QJY589829:QJY655360 QTU589829:QTU655360 RDQ589829:RDQ655360 RNM589829:RNM655360 RXI589829:RXI655360 SHE589829:SHE655360 SRA589829:SRA655360 TAW589829:TAW655360 TKS589829:TKS655360 TUO589829:TUO655360 UEK589829:UEK655360 UOG589829:UOG655360 UYC589829:UYC655360 VHY589829:VHY655360 VRU589829:VRU655360 WBQ589829:WBQ655360 WLM589829:WLM655360 WVI589829:WVI655360 A655365:A720896 IW655365:IW720896 SS655365:SS720896 ACO655365:ACO720896 AMK655365:AMK720896 AWG655365:AWG720896 BGC655365:BGC720896 BPY655365:BPY720896 BZU655365:BZU720896 CJQ655365:CJQ720896 CTM655365:CTM720896 DDI655365:DDI720896 DNE655365:DNE720896 DXA655365:DXA720896 EGW655365:EGW720896 EQS655365:EQS720896 FAO655365:FAO720896 FKK655365:FKK720896 FUG655365:FUG720896 GEC655365:GEC720896 GNY655365:GNY720896 GXU655365:GXU720896 HHQ655365:HHQ720896 HRM655365:HRM720896 IBI655365:IBI720896 ILE655365:ILE720896 IVA655365:IVA720896 JEW655365:JEW720896 JOS655365:JOS720896 JYO655365:JYO720896 KIK655365:KIK720896 KSG655365:KSG720896 LCC655365:LCC720896 LLY655365:LLY720896 LVU655365:LVU720896 MFQ655365:MFQ720896 MPM655365:MPM720896 MZI655365:MZI720896 NJE655365:NJE720896 NTA655365:NTA720896 OCW655365:OCW720896 OMS655365:OMS720896 OWO655365:OWO720896 PGK655365:PGK720896 PQG655365:PQG720896 QAC655365:QAC720896 QJY655365:QJY720896 QTU655365:QTU720896 RDQ655365:RDQ720896 RNM655365:RNM720896 RXI655365:RXI720896 SHE655365:SHE720896 SRA655365:SRA720896 TAW655365:TAW720896 TKS655365:TKS720896 TUO655365:TUO720896 UEK655365:UEK720896 UOG655365:UOG720896 UYC655365:UYC720896 VHY655365:VHY720896 VRU655365:VRU720896 WBQ655365:WBQ720896 WLM655365:WLM720896 WVI655365:WVI720896 A720901:A786432 IW720901:IW786432 SS720901:SS786432 ACO720901:ACO786432 AMK720901:AMK786432 AWG720901:AWG786432 BGC720901:BGC786432 BPY720901:BPY786432 BZU720901:BZU786432 CJQ720901:CJQ786432 CTM720901:CTM786432 DDI720901:DDI786432 DNE720901:DNE786432 DXA720901:DXA786432 EGW720901:EGW786432 EQS720901:EQS786432 FAO720901:FAO786432 FKK720901:FKK786432 FUG720901:FUG786432 GEC720901:GEC786432 GNY720901:GNY786432 GXU720901:GXU786432 HHQ720901:HHQ786432 HRM720901:HRM786432 IBI720901:IBI786432 ILE720901:ILE786432 IVA720901:IVA786432 JEW720901:JEW786432 JOS720901:JOS786432 JYO720901:JYO786432 KIK720901:KIK786432 KSG720901:KSG786432 LCC720901:LCC786432 LLY720901:LLY786432 LVU720901:LVU786432 MFQ720901:MFQ786432 MPM720901:MPM786432 MZI720901:MZI786432 NJE720901:NJE786432 NTA720901:NTA786432 OCW720901:OCW786432 OMS720901:OMS786432 OWO720901:OWO786432 PGK720901:PGK786432 PQG720901:PQG786432 QAC720901:QAC786432 QJY720901:QJY786432 QTU720901:QTU786432 RDQ720901:RDQ786432 RNM720901:RNM786432 RXI720901:RXI786432 SHE720901:SHE786432 SRA720901:SRA786432 TAW720901:TAW786432 TKS720901:TKS786432 TUO720901:TUO786432 UEK720901:UEK786432 UOG720901:UOG786432 UYC720901:UYC786432 VHY720901:VHY786432 VRU720901:VRU786432 WBQ720901:WBQ786432 WLM720901:WLM786432 WVI720901:WVI786432 A786437:A851968 IW786437:IW851968 SS786437:SS851968 ACO786437:ACO851968 AMK786437:AMK851968 AWG786437:AWG851968 BGC786437:BGC851968 BPY786437:BPY851968 BZU786437:BZU851968 CJQ786437:CJQ851968 CTM786437:CTM851968 DDI786437:DDI851968 DNE786437:DNE851968 DXA786437:DXA851968 EGW786437:EGW851968 EQS786437:EQS851968 FAO786437:FAO851968 FKK786437:FKK851968 FUG786437:FUG851968 GEC786437:GEC851968 GNY786437:GNY851968 GXU786437:GXU851968 HHQ786437:HHQ851968 HRM786437:HRM851968 IBI786437:IBI851968 ILE786437:ILE851968 IVA786437:IVA851968 JEW786437:JEW851968 JOS786437:JOS851968 JYO786437:JYO851968 KIK786437:KIK851968 KSG786437:KSG851968 LCC786437:LCC851968 LLY786437:LLY851968 LVU786437:LVU851968 MFQ786437:MFQ851968 MPM786437:MPM851968 MZI786437:MZI851968 NJE786437:NJE851968 NTA786437:NTA851968 OCW786437:OCW851968 OMS786437:OMS851968 OWO786437:OWO851968 PGK786437:PGK851968 PQG786437:PQG851968 QAC786437:QAC851968 QJY786437:QJY851968 QTU786437:QTU851968 RDQ786437:RDQ851968 RNM786437:RNM851968 RXI786437:RXI851968 SHE786437:SHE851968 SRA786437:SRA851968 TAW786437:TAW851968 TKS786437:TKS851968 TUO786437:TUO851968 UEK786437:UEK851968 UOG786437:UOG851968 UYC786437:UYC851968 VHY786437:VHY851968 VRU786437:VRU851968 WBQ786437:WBQ851968 WLM786437:WLM851968 WVI786437:WVI851968 A851973:A917504 IW851973:IW917504 SS851973:SS917504 ACO851973:ACO917504 AMK851973:AMK917504 AWG851973:AWG917504 BGC851973:BGC917504 BPY851973:BPY917504 BZU851973:BZU917504 CJQ851973:CJQ917504 CTM851973:CTM917504 DDI851973:DDI917504 DNE851973:DNE917504 DXA851973:DXA917504 EGW851973:EGW917504 EQS851973:EQS917504 FAO851973:FAO917504 FKK851973:FKK917504 FUG851973:FUG917504 GEC851973:GEC917504 GNY851973:GNY917504 GXU851973:GXU917504 HHQ851973:HHQ917504 HRM851973:HRM917504 IBI851973:IBI917504 ILE851973:ILE917504 IVA851973:IVA917504 JEW851973:JEW917504 JOS851973:JOS917504 JYO851973:JYO917504 KIK851973:KIK917504 KSG851973:KSG917504 LCC851973:LCC917504 LLY851973:LLY917504 LVU851973:LVU917504 MFQ851973:MFQ917504 MPM851973:MPM917504 MZI851973:MZI917504 NJE851973:NJE917504 NTA851973:NTA917504 OCW851973:OCW917504 OMS851973:OMS917504 OWO851973:OWO917504 PGK851973:PGK917504 PQG851973:PQG917504 QAC851973:QAC917504 QJY851973:QJY917504 QTU851973:QTU917504 RDQ851973:RDQ917504 RNM851973:RNM917504 RXI851973:RXI917504 SHE851973:SHE917504 SRA851973:SRA917504 TAW851973:TAW917504 TKS851973:TKS917504 TUO851973:TUO917504 UEK851973:UEK917504 UOG851973:UOG917504 UYC851973:UYC917504 VHY851973:VHY917504 VRU851973:VRU917504 WBQ851973:WBQ917504 WLM851973:WLM917504 WVI851973:WVI917504 A917509:A983040 IW917509:IW983040 SS917509:SS983040 ACO917509:ACO983040 AMK917509:AMK983040 AWG917509:AWG983040 BGC917509:BGC983040 BPY917509:BPY983040 BZU917509:BZU983040 CJQ917509:CJQ983040 CTM917509:CTM983040 DDI917509:DDI983040 DNE917509:DNE983040 DXA917509:DXA983040 EGW917509:EGW983040 EQS917509:EQS983040 FAO917509:FAO983040 FKK917509:FKK983040 FUG917509:FUG983040 GEC917509:GEC983040 GNY917509:GNY983040 GXU917509:GXU983040 HHQ917509:HHQ983040 HRM917509:HRM983040 IBI917509:IBI983040 ILE917509:ILE983040 IVA917509:IVA983040 JEW917509:JEW983040 JOS917509:JOS983040 JYO917509:JYO983040 KIK917509:KIK983040 KSG917509:KSG983040 LCC917509:LCC983040 LLY917509:LLY983040 LVU917509:LVU983040 MFQ917509:MFQ983040 MPM917509:MPM983040 MZI917509:MZI983040 NJE917509:NJE983040 NTA917509:NTA983040 OCW917509:OCW983040 OMS917509:OMS983040 OWO917509:OWO983040 PGK917509:PGK983040 PQG917509:PQG983040 QAC917509:QAC983040 QJY917509:QJY983040 QTU917509:QTU983040 RDQ917509:RDQ983040 RNM917509:RNM983040 RXI917509:RXI983040 SHE917509:SHE983040 SRA917509:SRA983040 TAW917509:TAW983040 TKS917509:TKS983040 TUO917509:TUO983040 UEK917509:UEK983040 UOG917509:UOG983040 UYC917509:UYC983040 VHY917509:VHY983040 VRU917509:VRU983040 WBQ917509:WBQ983040 WLM917509:WLM983040 WVI917509:WVI983040 A983045:A1048576 IW983045:IW1048576 SS983045:SS1048576 ACO983045:ACO1048576 AMK983045:AMK1048576 AWG983045:AWG1048576 BGC983045:BGC1048576 BPY983045:BPY1048576 BZU983045:BZU1048576 CJQ983045:CJQ1048576 CTM983045:CTM1048576 DDI983045:DDI1048576 DNE983045:DNE1048576 DXA983045:DXA1048576 EGW983045:EGW1048576 EQS983045:EQS1048576 FAO983045:FAO1048576 FKK983045:FKK1048576 FUG983045:FUG1048576 GEC983045:GEC1048576 GNY983045:GNY1048576 GXU983045:GXU1048576 HHQ983045:HHQ1048576 HRM983045:HRM1048576 IBI983045:IBI1048576 ILE983045:ILE1048576 IVA983045:IVA1048576 JEW983045:JEW1048576 JOS983045:JOS1048576 JYO983045:JYO1048576 KIK983045:KIK1048576 KSG983045:KSG1048576 LCC983045:LCC1048576 LLY983045:LLY1048576 LVU983045:LVU1048576 MFQ983045:MFQ1048576 MPM983045:MPM1048576 MZI983045:MZI1048576 NJE983045:NJE1048576 NTA983045:NTA1048576 OCW983045:OCW1048576 OMS983045:OMS1048576 OWO983045:OWO1048576 PGK983045:PGK1048576 PQG983045:PQG1048576 QAC983045:QAC1048576 QJY983045:QJY1048576 QTU983045:QTU1048576 RDQ983045:RDQ1048576 RNM983045:RNM1048576 RXI983045:RXI1048576 SHE983045:SHE1048576 SRA983045:SRA1048576 TAW983045:TAW1048576 TKS983045:TKS1048576 TUO983045:TUO1048576 UEK983045:UEK1048576 UOG983045:UOG1048576 UYC983045:UYC1048576 VHY983045:VHY1048576 VRU983045:VRU1048576 WBQ983045:WBQ1048576 WLM983045:WLM1048576 WVI983045:WVI1048576">
+      <formula1>"-"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>